<commit_message>
commit intermédiaire de fin de semaine
</commit_message>
<xml_diff>
--- a/Liste de dons LG Apocalypse.xlsx
+++ b/Liste de dons LG Apocalypse.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8C6A5C60-E91F-490D-BB15-FED2150B4114}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{414E4CC9-A408-4207-968D-236C41C2FC72}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3370" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3406" uniqueCount="885">
   <si>
     <t>Liste</t>
   </si>
@@ -2649,10 +2649,49 @@
     <t>Esquive</t>
   </si>
   <si>
-    <t>Ragnarok</t>
-  </si>
-  <si>
     <t>Férocité, combat et combat</t>
+  </si>
+  <si>
+    <t>Permet de passer d'une action aggressive à une action défensive gratuitement</t>
+  </si>
+  <si>
+    <t>1 jour</t>
+  </si>
+  <si>
+    <t>Férocité ?</t>
+  </si>
+  <si>
+    <t>Ragnarok ?</t>
+  </si>
+  <si>
+    <t>Le LG semble plus grand et térrifiant</t>
+  </si>
+  <si>
+    <t>Charisme + Initimidation</t>
+  </si>
+  <si>
+    <t>Ragnarok?</t>
+  </si>
+  <si>
+    <t>Les crocs du LG exhalent une fumée bleue et sont transformées en glace dure. Les plaies infligées gangrènent</t>
+  </si>
+  <si>
+    <t>Astuce + Survie</t>
+  </si>
+  <si>
+    <t>Ralenti les ennemis qui fuient pour les rattraper</t>
+  </si>
+  <si>
+    <t>Grondement bestion qui terrifie et intimide</t>
+  </si>
+  <si>
+    <t>Renforme la peau du LG pour augmenter son absorption</t>
+  </si>
+  <si>
+    <t>Augmente la force du LG</t>
+  </si>
+  <si>
+    <t>Redirige la douleur de ses blessures à ceux qui les lui ont infligées</t>
   </si>
 </sst>
 </file>
@@ -8375,7 +8414,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{477637CD-FD25-47E8-A7D2-A30D4A046A9C}" name="TablaDinámica1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{477637CD-FD25-47E8-A7D2-A30D4A046A9C}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:W58" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -11070,7 +11109,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E270" sqref="E270"/>
+      <selection pane="bottomLeft" activeCell="E274" sqref="E274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11141,7 +11180,7 @@
         <v>560</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D2)=1,"Oui","Non")</f>
+        <f t="shared" ref="F2:F65" si="0">IF(COUNTIF(D:D,"="&amp;D2)=1,"Oui","Non")</f>
         <v>Oui</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -11177,7 +11216,7 @@
         <v>491</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D3)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -11213,7 +11252,7 @@
         <v>311</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D4)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -11249,7 +11288,7 @@
         <v>560</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D5)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -11285,7 +11324,7 @@
         <v>687</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D6)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -11321,7 +11360,7 @@
         <v>296</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D7)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -11357,7 +11396,7 @@
         <v>560</v>
       </c>
       <c r="F8" s="2" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D8)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -11393,7 +11432,7 @@
         <v>595</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D9)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -11429,7 +11468,7 @@
         <v>595</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D10)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -11465,7 +11504,7 @@
         <v>595</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D11)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -11501,7 +11540,7 @@
         <v>399</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D12)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -11537,7 +11576,7 @@
         <v>305</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D13)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -11573,7 +11612,7 @@
         <v>395</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D14)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -11609,7 +11648,7 @@
         <v>402</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D15)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -11645,7 +11684,7 @@
         <v>389</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D16)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -11681,7 +11720,7 @@
         <v>93</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D17)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -11717,7 +11756,7 @@
         <v>595</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D18)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -11753,7 +11792,7 @@
         <v>560</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D19)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -11789,7 +11828,7 @@
         <v>595</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D20)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -11825,7 +11864,7 @@
         <v>560</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D21)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -11861,7 +11900,7 @@
         <v>496</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D22)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -11897,7 +11936,7 @@
         <v>311</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D23)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -11933,7 +11972,7 @@
         <v>520</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D24)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -11969,7 +12008,7 @@
         <v>520</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D25)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -12005,7 +12044,7 @@
         <v>412</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D26)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G26" s="3" t="s">
@@ -12041,7 +12080,7 @@
         <v>520</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D27)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -12074,7 +12113,7 @@
         <v>402</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D28)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -12110,7 +12149,7 @@
         <v>422</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D29)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G29" s="3" t="s">
@@ -12143,7 +12182,7 @@
         <v>412</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D30)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -12179,7 +12218,7 @@
         <v>427</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D31)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G31" s="3" t="s">
@@ -12215,7 +12254,7 @@
         <v>395</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D32)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -12251,7 +12290,7 @@
         <v>422</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D33)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G33" s="3" t="s">
@@ -12287,7 +12326,7 @@
         <v>520</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D34)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -12323,7 +12362,7 @@
         <v>520</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D35)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -12359,7 +12398,7 @@
         <v>496</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D36)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -12395,7 +12434,7 @@
         <v>422</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D37)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G37" s="3" t="s">
@@ -12431,7 +12470,7 @@
         <v>520</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D38)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -12467,7 +12506,7 @@
         <v>402</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D39)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G39" s="3" t="s">
@@ -12503,7 +12542,7 @@
         <v>407</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D40)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -12539,7 +12578,7 @@
         <v>422</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D41)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G41" s="3" t="s">
@@ -12575,7 +12614,7 @@
         <v>573</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D42)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G42" s="3" t="s">
@@ -12611,7 +12650,7 @@
         <v>520</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D43)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G43" s="3" t="s">
@@ -12647,7 +12686,7 @@
         <v>594</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D44)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -12683,7 +12722,7 @@
         <v>412</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D45)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G45" s="3" t="s">
@@ -12719,7 +12758,7 @@
         <v>573</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D46)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G46" s="3" t="s">
@@ -12755,7 +12794,7 @@
         <v>576</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D47)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G47" s="3" t="s">
@@ -12791,7 +12830,7 @@
         <v>407</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D48)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G48" s="3" t="s">
@@ -12827,7 +12866,7 @@
         <v>412</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D49)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G49" s="3" t="s">
@@ -12863,7 +12902,7 @@
         <v>412</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D50)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G50" s="3" t="s">
@@ -12899,7 +12938,7 @@
         <v>296</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D51)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G51" s="3" t="s">
@@ -12935,7 +12974,7 @@
         <v>573</v>
       </c>
       <c r="F52" s="2" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D52)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G52" s="4" t="s">
@@ -12971,7 +13010,7 @@
         <v>520</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D53)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G53" s="3" t="s">
@@ -13007,7 +13046,7 @@
         <v>412</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D54)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G54" s="3" t="s">
@@ -13043,7 +13082,7 @@
         <v>402</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D55)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G55" s="3" t="s">
@@ -13079,7 +13118,7 @@
         <v>422</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D56)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G56" s="3" t="s">
@@ -13115,7 +13154,7 @@
         <v>573</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D57)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G57" s="3" t="s">
@@ -13151,7 +13190,7 @@
         <v>595</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D58)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G58" s="3" t="s">
@@ -13187,7 +13226,7 @@
         <v>425</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D59)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G59" s="3" t="s">
@@ -13223,7 +13262,7 @@
         <v>311</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D60)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G60" s="3" t="s">
@@ -13259,7 +13298,7 @@
         <v>633</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D61)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G61" s="3" t="s">
@@ -13295,7 +13334,7 @@
         <v>427</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D62)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Non</v>
       </c>
       <c r="G62" s="3" t="s">
@@ -13331,7 +13370,7 @@
         <v>592</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D63)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G63" s="3" t="s">
@@ -13367,7 +13406,7 @@
         <v>395</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D64)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G64" s="3" t="s">
@@ -13403,7 +13442,7 @@
         <v>427</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D65)=1,"Oui","Non")</f>
+        <f t="shared" si="0"/>
         <v>Oui</v>
       </c>
       <c r="G65" s="3" t="s">
@@ -13439,7 +13478,7 @@
         <v>592</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D66)=1,"Oui","Non")</f>
+        <f t="shared" ref="F66:F129" si="1">IF(COUNTIF(D:D,"="&amp;D66)=1,"Oui","Non")</f>
         <v>Oui</v>
       </c>
       <c r="G66" s="3" t="s">
@@ -13475,7 +13514,7 @@
         <v>592</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D67)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G67" s="3" t="s">
@@ -13511,7 +13550,7 @@
         <v>427</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D68)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G68" s="3" t="s">
@@ -13547,7 +13586,7 @@
         <v>573</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D69)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G69" s="3" t="s">
@@ -13583,7 +13622,7 @@
         <v>592</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D70)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G70" s="3" t="s">
@@ -13619,7 +13658,7 @@
         <v>592</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D71)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G71" s="3" t="s">
@@ -13655,7 +13694,7 @@
         <v>576</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D72)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G72" s="3" t="s">
@@ -13691,7 +13730,7 @@
         <v>296</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D73)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G73" s="3" t="s">
@@ -13727,7 +13766,7 @@
         <v>576</v>
       </c>
       <c r="F74" s="2" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D74)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G74" s="4" t="s">
@@ -13763,7 +13802,7 @@
         <v>402</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D75)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G75" s="3" t="s">
@@ -13799,7 +13838,7 @@
         <v>595</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D76)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G76" s="3" t="s">
@@ -13835,7 +13874,7 @@
         <v>422</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D77)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G77" s="3" t="s">
@@ -13871,7 +13910,7 @@
         <v>592</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D78)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G78" s="3" t="s">
@@ -13907,7 +13946,7 @@
         <v>402</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D79)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G79" s="3" t="s">
@@ -13943,7 +13982,7 @@
         <v>592</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D80)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G80" s="3" t="s">
@@ -13979,7 +14018,7 @@
         <v>592</v>
       </c>
       <c r="F81" s="2" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D81)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G81" s="4" t="s">
@@ -14015,7 +14054,7 @@
         <v>652</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D82)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G82" s="3" t="s">
@@ -14051,7 +14090,7 @@
         <v>407</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D83)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G83" s="3" t="s">
@@ -14087,7 +14126,7 @@
         <v>93</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D84)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G84" s="3" t="s">
@@ -14123,7 +14162,7 @@
         <v>412</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D85)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G85" s="3" t="s">
@@ -14159,7 +14198,7 @@
         <v>846</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D86)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G86" s="3" t="s">
@@ -14195,7 +14234,7 @@
         <v>93</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D87)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G87" s="3" t="s">
@@ -14231,7 +14270,7 @@
         <v>93</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D88)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G88" s="3" t="s">
@@ -14267,7 +14306,7 @@
         <v>93</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D89)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G89" s="3" t="s">
@@ -14303,7 +14342,7 @@
         <v>422</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D90)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G90" s="3" t="s">
@@ -14339,7 +14378,7 @@
         <v>427</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D91)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G91" s="3" t="s">
@@ -14375,7 +14414,7 @@
         <v>93</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D92)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G92" s="3" t="s">
@@ -14411,7 +14450,7 @@
         <v>652</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D93)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G93" s="3" t="s">
@@ -14447,7 +14486,7 @@
         <v>407</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D94)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G94" s="3" t="s">
@@ -14483,7 +14522,7 @@
         <v>93</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D95)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G95" s="3" t="s">
@@ -14519,7 +14558,7 @@
         <v>93</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D96)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G96" s="3" t="s">
@@ -14555,7 +14594,7 @@
         <v>652</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D97)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G97" s="3" t="s">
@@ -14591,7 +14630,7 @@
         <v>652</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D98)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G98" s="3" t="s">
@@ -14627,7 +14666,7 @@
         <v>407</v>
       </c>
       <c r="F99" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D99)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G99" s="3" t="s">
@@ -14663,7 +14702,7 @@
         <v>422</v>
       </c>
       <c r="F100" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D100)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G100" s="3" t="s">
@@ -14699,7 +14738,7 @@
         <v>298</v>
       </c>
       <c r="F101" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D101)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G101" s="3" t="s">
@@ -14735,7 +14774,7 @@
         <v>407</v>
       </c>
       <c r="F102" s="2" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D102)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G102" s="4" t="s">
@@ -14771,7 +14810,7 @@
         <v>678</v>
       </c>
       <c r="F103" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D103)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G103" s="3" t="s">
@@ -14807,7 +14846,7 @@
         <v>412</v>
       </c>
       <c r="F104" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D104)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G104" s="3" t="s">
@@ -14843,7 +14882,7 @@
         <v>687</v>
       </c>
       <c r="F105" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D105)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G105" s="3" t="s">
@@ -14879,7 +14918,7 @@
         <v>389</v>
       </c>
       <c r="F106" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D106)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G106" s="3" t="s">
@@ -14915,7 +14954,7 @@
         <v>678</v>
       </c>
       <c r="F107" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D107)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G107" s="3" t="s">
@@ -14951,7 +14990,7 @@
         <v>687</v>
       </c>
       <c r="F108" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D108)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G108" s="3" t="s">
@@ -14987,7 +15026,7 @@
         <v>687</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D109)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G109" s="3" t="s">
@@ -15023,7 +15062,7 @@
         <v>488</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D110)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G110" s="3" t="s">
@@ -15059,7 +15098,7 @@
         <v>687</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D111)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G111" s="3" t="s">
@@ -15095,7 +15134,7 @@
         <v>678</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D112)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G112" s="3" t="s">
@@ -15131,7 +15170,7 @@
         <v>422</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D113)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G113" s="3" t="s">
@@ -15167,7 +15206,7 @@
         <v>439</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D114)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G114" s="3" t="s">
@@ -15203,7 +15242,7 @@
         <v>412</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D115)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G115" s="3" t="s">
@@ -15239,7 +15278,7 @@
         <v>422</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D116)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G116" s="3" t="s">
@@ -15275,7 +15314,7 @@
         <v>687</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D117)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G117" s="3" t="s">
@@ -15311,7 +15350,7 @@
         <v>678</v>
       </c>
       <c r="F118" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D118)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G118" s="3" t="s">
@@ -15347,7 +15386,7 @@
         <v>412</v>
       </c>
       <c r="F119" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D119)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G119" s="3" t="s">
@@ -15380,7 +15419,7 @@
         <v>311</v>
       </c>
       <c r="F120" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D120)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G120" s="3" t="s">
@@ -15416,7 +15455,7 @@
         <v>594</v>
       </c>
       <c r="F121" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D121)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G121" s="3" t="s">
@@ -15452,7 +15491,7 @@
         <v>678</v>
       </c>
       <c r="F122" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D122)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G122" s="3" t="s">
@@ -15488,7 +15527,7 @@
         <v>703</v>
       </c>
       <c r="F123" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D123)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G123" s="3" t="s">
@@ -15524,7 +15563,7 @@
         <v>703</v>
       </c>
       <c r="F124" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D124)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G124" s="3" t="s">
@@ -15560,7 +15599,7 @@
         <v>422</v>
       </c>
       <c r="F125" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D125)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G125" s="3" t="s">
@@ -15596,7 +15635,7 @@
         <v>712</v>
       </c>
       <c r="F126" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D126)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G126" s="3" t="s">
@@ -15632,7 +15671,7 @@
         <v>412</v>
       </c>
       <c r="F127" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D127)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G127" s="3" t="s">
@@ -15668,7 +15707,7 @@
         <v>703</v>
       </c>
       <c r="F128" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D128)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Oui</v>
       </c>
       <c r="G128" s="3" t="s">
@@ -15704,7 +15743,7 @@
         <v>298</v>
       </c>
       <c r="F129" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D129)=1,"Oui","Non")</f>
+        <f t="shared" si="1"/>
         <v>Non</v>
       </c>
       <c r="G129" s="3" t="s">
@@ -15740,7 +15779,7 @@
         <v>703</v>
       </c>
       <c r="F130" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D130)=1,"Oui","Non")</f>
+        <f t="shared" ref="F130:F193" si="2">IF(COUNTIF(D:D,"="&amp;D130)=1,"Oui","Non")</f>
         <v>Oui</v>
       </c>
       <c r="G130" s="3" t="s">
@@ -15776,7 +15815,7 @@
         <v>703</v>
       </c>
       <c r="F131" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D131)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G131" s="3" t="s">
@@ -15812,7 +15851,7 @@
         <v>712</v>
       </c>
       <c r="F132" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D132)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G132" s="3" t="s">
@@ -15848,7 +15887,7 @@
         <v>703</v>
       </c>
       <c r="F133" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D133)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G133" s="3" t="s">
@@ -15884,7 +15923,7 @@
         <v>703</v>
       </c>
       <c r="F134" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D134)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G134" s="3" t="s">
@@ -15920,7 +15959,7 @@
         <v>703</v>
       </c>
       <c r="F135" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D135)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G135" s="3" t="s">
@@ -15956,7 +15995,7 @@
         <v>712</v>
       </c>
       <c r="F136" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D136)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G136" s="3" t="s">
@@ -15992,7 +16031,7 @@
         <v>712</v>
       </c>
       <c r="F137" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D137)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G137" s="3" t="s">
@@ -16028,7 +16067,7 @@
         <v>422</v>
       </c>
       <c r="F138" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D138)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G138" s="3" t="s">
@@ -16064,7 +16103,7 @@
         <v>712</v>
       </c>
       <c r="F139" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D139)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G139" s="3" t="s">
@@ -16100,7 +16139,7 @@
         <v>633</v>
       </c>
       <c r="F140" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D140)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G140" s="3" t="s">
@@ -16136,7 +16175,7 @@
         <v>712</v>
       </c>
       <c r="F141" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D141)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G141" s="3" t="s">
@@ -16172,7 +16211,7 @@
         <v>594</v>
       </c>
       <c r="F142" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D142)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G142" s="3" t="s">
@@ -16208,7 +16247,7 @@
         <v>452</v>
       </c>
       <c r="F143" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D143)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G143" s="3" t="s">
@@ -16244,7 +16283,7 @@
         <v>452</v>
       </c>
       <c r="F144" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D144)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G144" s="3" t="s">
@@ -16280,7 +16319,7 @@
         <v>797</v>
       </c>
       <c r="F145" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D145)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G145" s="3" t="s">
@@ -16316,7 +16355,7 @@
         <v>783</v>
       </c>
       <c r="F146" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D146)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G146" s="3" t="s">
@@ -16352,7 +16391,7 @@
         <v>768</v>
       </c>
       <c r="F147" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D147)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G147" s="3" t="s">
@@ -16388,7 +16427,7 @@
         <v>769</v>
       </c>
       <c r="F148" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D148)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G148" s="3" t="s">
@@ -16424,7 +16463,7 @@
         <v>768</v>
       </c>
       <c r="F149" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D149)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G149" s="3" t="s">
@@ -16460,7 +16499,7 @@
         <v>412</v>
       </c>
       <c r="F150" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D150)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G150" s="3" t="s">
@@ -16496,7 +16535,7 @@
         <v>769</v>
       </c>
       <c r="F151" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D151)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G151" s="3" t="s">
@@ -16532,7 +16571,7 @@
         <v>769</v>
       </c>
       <c r="F152" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D152)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G152" s="3" t="s">
@@ -16568,7 +16607,7 @@
         <v>452</v>
       </c>
       <c r="F153" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D153)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G153" s="3" t="s">
@@ -16604,7 +16643,7 @@
         <v>452</v>
       </c>
       <c r="F154" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D154)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G154" s="3" t="s">
@@ -16640,7 +16679,7 @@
         <v>845</v>
       </c>
       <c r="F155" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D155)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G155" s="3" t="s">
@@ -16676,7 +16715,7 @@
         <v>402</v>
       </c>
       <c r="F156" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D156)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G156" s="3" t="s">
@@ -16712,7 +16751,7 @@
         <v>769</v>
       </c>
       <c r="F157" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D157)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G157" s="3" t="s">
@@ -16748,7 +16787,7 @@
         <v>768</v>
       </c>
       <c r="F158" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D158)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G158" s="3" t="s">
@@ -16784,7 +16823,7 @@
         <v>452</v>
       </c>
       <c r="F159" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D159)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G159" s="3" t="s">
@@ -16820,7 +16859,7 @@
         <v>311</v>
       </c>
       <c r="F160" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D160)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G160" s="3" t="s">
@@ -16856,7 +16895,7 @@
         <v>488</v>
       </c>
       <c r="F161" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D161)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G161" s="3" t="s">
@@ -16892,7 +16931,7 @@
         <v>845</v>
       </c>
       <c r="F162" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D162)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G162" s="3" t="s">
@@ -16928,7 +16967,7 @@
         <v>576</v>
       </c>
       <c r="F163" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D163)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G163" s="3" t="s">
@@ -16964,7 +17003,7 @@
         <v>412</v>
       </c>
       <c r="F164" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D164)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G164" s="3" t="s">
@@ -17000,7 +17039,7 @@
         <v>427</v>
       </c>
       <c r="F165" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D165)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G165" s="3" t="s">
@@ -17036,7 +17075,7 @@
         <v>757</v>
       </c>
       <c r="F166" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D166)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G166" s="3" t="s">
@@ -17072,7 +17111,7 @@
         <v>576</v>
       </c>
       <c r="F167" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D167)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G167" s="3" t="s">
@@ -17108,7 +17147,7 @@
         <v>576</v>
       </c>
       <c r="F168" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D168)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G168" s="3" t="s">
@@ -17144,7 +17183,7 @@
         <v>576</v>
       </c>
       <c r="F169" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D169)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G169" s="3" t="s">
@@ -17180,7 +17219,7 @@
         <v>427</v>
       </c>
       <c r="F170" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D170)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G170" s="3" t="s">
@@ -17216,7 +17255,7 @@
         <v>560</v>
       </c>
       <c r="F171" s="2" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D171)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G171" s="4" t="s">
@@ -17252,7 +17291,7 @@
         <v>576</v>
       </c>
       <c r="F172" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D172)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G172" s="3" t="s">
@@ -17288,7 +17327,7 @@
         <v>316</v>
       </c>
       <c r="F173" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D173)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G173" s="3" t="s">
@@ -17324,7 +17363,7 @@
         <v>576</v>
       </c>
       <c r="F174" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D174)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G174" s="3" t="s">
@@ -17360,7 +17399,7 @@
         <v>757</v>
       </c>
       <c r="F175" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D175)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G175" s="3" t="s">
@@ -17396,7 +17435,7 @@
         <v>422</v>
       </c>
       <c r="F176" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D176)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G176" s="3" t="s">
@@ -17432,7 +17471,7 @@
         <v>757</v>
       </c>
       <c r="F177" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D177)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G177" s="3" t="s">
@@ -17468,7 +17507,7 @@
         <v>757</v>
       </c>
       <c r="F178" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D178)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G178" s="3" t="s">
@@ -17504,7 +17543,7 @@
         <v>576</v>
       </c>
       <c r="F179" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D179)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G179" s="3" t="s">
@@ -17540,7 +17579,7 @@
         <v>407</v>
       </c>
       <c r="F180" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D180)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G180" s="3" t="s">
@@ -17576,7 +17615,7 @@
         <v>652</v>
       </c>
       <c r="F181" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D181)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G181" s="3" t="s">
@@ -17612,7 +17651,7 @@
         <v>422</v>
       </c>
       <c r="F182" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D182)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G182" s="3" t="s">
@@ -17648,7 +17687,7 @@
         <v>496</v>
       </c>
       <c r="F183" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D183)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G183" s="3" t="s">
@@ -17684,7 +17723,7 @@
         <v>770</v>
       </c>
       <c r="F184" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D184)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G184" s="3" t="s">
@@ -17720,7 +17759,7 @@
         <v>783</v>
       </c>
       <c r="F185" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D185)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G185" s="3" t="s">
@@ -17756,7 +17795,7 @@
         <v>488</v>
       </c>
       <c r="F186" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D186)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G186" s="3" t="s">
@@ -17792,7 +17831,7 @@
         <v>412</v>
       </c>
       <c r="F187" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D187)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Non</v>
       </c>
       <c r="G187" s="3" t="s">
@@ -17828,7 +17867,7 @@
         <v>488</v>
       </c>
       <c r="F188" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D188)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G188" s="3" t="s">
@@ -17864,7 +17903,7 @@
         <v>652</v>
       </c>
       <c r="F189" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D189)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G189" s="3" t="s">
@@ -17900,7 +17939,7 @@
         <v>488</v>
       </c>
       <c r="F190" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D190)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G190" s="3" t="s">
@@ -17936,7 +17975,7 @@
         <v>576</v>
       </c>
       <c r="F191" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D191)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G191" s="3" t="s">
@@ -17972,7 +18011,7 @@
         <v>399</v>
       </c>
       <c r="F192" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D192)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G192" s="3" t="s">
@@ -18008,7 +18047,7 @@
         <v>412</v>
       </c>
       <c r="F193" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D193)=1,"Oui","Non")</f>
+        <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
       <c r="G193" s="3" t="s">
@@ -18044,7 +18083,7 @@
         <v>783</v>
       </c>
       <c r="F194" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D194)=1,"Oui","Non")</f>
+        <f t="shared" ref="F194:F257" si="3">IF(COUNTIF(D:D,"="&amp;D194)=1,"Oui","Non")</f>
         <v>Oui</v>
       </c>
       <c r="G194" s="3" t="s">
@@ -18080,7 +18119,7 @@
         <v>783</v>
       </c>
       <c r="F195" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D195)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G195" s="3" t="s">
@@ -18116,7 +18155,7 @@
         <v>412</v>
       </c>
       <c r="F196" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D196)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G196" s="3" t="s">
@@ -18152,7 +18191,7 @@
         <v>389</v>
       </c>
       <c r="F197" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D197)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G197" s="3" t="s">
@@ -18188,7 +18227,7 @@
         <v>783</v>
       </c>
       <c r="F198" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D198)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G198" s="3" t="s">
@@ -18224,7 +18263,7 @@
         <v>783</v>
       </c>
       <c r="F199" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D199)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G199" s="3" t="s">
@@ -18260,7 +18299,7 @@
         <v>783</v>
       </c>
       <c r="F200" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D200)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G200" s="3" t="s">
@@ -18296,7 +18335,7 @@
         <v>488</v>
       </c>
       <c r="F201" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D201)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G201" s="3" t="s">
@@ -18332,7 +18371,7 @@
         <v>422</v>
       </c>
       <c r="F202" s="2" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D202)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G202" s="4" t="s">
@@ -18368,7 +18407,7 @@
         <v>797</v>
       </c>
       <c r="F203" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D203)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G203" s="3" t="s">
@@ -18404,7 +18443,7 @@
         <v>797</v>
       </c>
       <c r="F204" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D204)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G204" s="3" t="s">
@@ -18440,7 +18479,7 @@
         <v>305</v>
       </c>
       <c r="F205" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D205)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G205" s="3" t="s">
@@ -18476,7 +18515,7 @@
         <v>422</v>
       </c>
       <c r="F206" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D206)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G206" s="3" t="s">
@@ -18512,7 +18551,7 @@
         <v>412</v>
       </c>
       <c r="F207" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D207)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G207" s="3" t="s">
@@ -18548,7 +18587,7 @@
         <v>389</v>
       </c>
       <c r="F208" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D208)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G208" s="3" t="s">
@@ -18584,7 +18623,7 @@
         <v>804</v>
       </c>
       <c r="F209" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D209)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G209" s="3" t="s">
@@ -18620,7 +18659,7 @@
         <v>402</v>
       </c>
       <c r="F210" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D210)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G210" s="3" t="s">
@@ -18656,7 +18695,7 @@
         <v>412</v>
       </c>
       <c r="F211" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D211)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G211" s="3" t="s">
@@ -18692,7 +18731,7 @@
         <v>804</v>
       </c>
       <c r="F212" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D212)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G212" s="3" t="s">
@@ -18728,7 +18767,7 @@
         <v>797</v>
       </c>
       <c r="F213" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D213)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G213" s="3" t="s">
@@ -18764,7 +18803,7 @@
         <v>452</v>
       </c>
       <c r="F214" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D214)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G214" s="3" t="s">
@@ -18800,7 +18839,7 @@
         <v>802</v>
       </c>
       <c r="F215" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D215)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G215" s="3" t="s">
@@ -18836,7 +18875,7 @@
         <v>452</v>
       </c>
       <c r="F216" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D216)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G216" s="3" t="s">
@@ -18872,7 +18911,7 @@
         <v>389</v>
       </c>
       <c r="F217" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D217)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G217" s="3" t="s">
@@ -18908,7 +18947,7 @@
         <v>797</v>
       </c>
       <c r="F218" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D218)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G218" s="3" t="s">
@@ -18944,7 +18983,7 @@
         <v>804</v>
       </c>
       <c r="F219" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D219)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G219" s="3" t="s">
@@ -18980,7 +19019,7 @@
         <v>422</v>
       </c>
       <c r="F220" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D220)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G220" s="3" t="s">
@@ -19016,7 +19055,7 @@
         <v>595</v>
       </c>
       <c r="F221" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D221)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G221" s="3" t="s">
@@ -19052,7 +19091,7 @@
         <v>757</v>
       </c>
       <c r="F222" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D222)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G222" s="3" t="s">
@@ -19088,7 +19127,7 @@
         <v>422</v>
       </c>
       <c r="F223" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D223)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G223" s="3" t="s">
@@ -19124,7 +19163,7 @@
         <v>846</v>
       </c>
       <c r="F224" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D224)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G224" s="3" t="s">
@@ -19160,7 +19199,7 @@
         <v>823</v>
       </c>
       <c r="F225" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D225)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G225" s="3" t="s">
@@ -19196,7 +19235,7 @@
         <v>389</v>
       </c>
       <c r="F226" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D226)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G226" s="3" t="s">
@@ -19232,7 +19271,7 @@
         <v>846</v>
       </c>
       <c r="F227" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D227)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G227" s="3" t="s">
@@ -19268,7 +19307,7 @@
         <v>389</v>
       </c>
       <c r="F228" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D228)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G228" s="3" t="s">
@@ -19304,7 +19343,7 @@
         <v>823</v>
       </c>
       <c r="F229" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D229)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G229" s="3" t="s">
@@ -19340,7 +19379,7 @@
         <v>823</v>
       </c>
       <c r="F230" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D230)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G230" s="3" t="s">
@@ -19376,7 +19415,7 @@
         <v>823</v>
       </c>
       <c r="F231" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D231)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G231" s="3" t="s">
@@ -19412,7 +19451,7 @@
         <v>846</v>
       </c>
       <c r="F232" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D232)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G232" s="3" t="s">
@@ -19448,7 +19487,7 @@
         <v>846</v>
       </c>
       <c r="F233" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D233)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G233" s="3" t="s">
@@ -19484,7 +19523,7 @@
         <v>595</v>
       </c>
       <c r="F234" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D234)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G234" s="3" t="s">
@@ -19520,7 +19559,7 @@
         <v>823</v>
       </c>
       <c r="F235" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D235)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G235" s="3" t="s">
@@ -19556,7 +19595,7 @@
         <v>846</v>
       </c>
       <c r="F236" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D236)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G236" s="3" t="s">
@@ -19592,7 +19631,7 @@
         <v>783</v>
       </c>
       <c r="F237" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D237)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G237" s="3" t="s">
@@ -19628,7 +19667,7 @@
         <v>594</v>
       </c>
       <c r="F238" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D238)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G238" s="3" t="s">
@@ -19664,7 +19703,7 @@
         <v>823</v>
       </c>
       <c r="F239" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D239)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G239" s="3" t="s">
@@ -19700,7 +19739,7 @@
         <v>425</v>
       </c>
       <c r="F240" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D240)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G240" s="3" t="s">
@@ -19736,7 +19775,7 @@
         <v>846</v>
       </c>
       <c r="F241" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D241)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G241" s="3" t="s">
@@ -19772,7 +19811,7 @@
         <v>422</v>
       </c>
       <c r="F242" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D242)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G242" s="3" t="s">
@@ -19808,7 +19847,7 @@
         <v>520</v>
       </c>
       <c r="F243" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D243)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G243" s="3" t="s">
@@ -19844,7 +19883,7 @@
         <v>868</v>
       </c>
       <c r="F244" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D244)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G244" s="3" t="s">
@@ -19880,7 +19919,7 @@
         <v>867</v>
       </c>
       <c r="F245" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D245)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G245" s="3" t="s">
@@ -19916,7 +19955,7 @@
         <v>687</v>
       </c>
       <c r="F246" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D246)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G246" s="3" t="s">
@@ -19952,7 +19991,7 @@
         <v>389</v>
       </c>
       <c r="F247" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D247)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G247" s="3" t="s">
@@ -19988,7 +20027,7 @@
         <v>869</v>
       </c>
       <c r="F248" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D248)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G248" s="3" t="s">
@@ -20024,7 +20063,7 @@
         <v>868</v>
       </c>
       <c r="F249" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D249)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G249" s="3" t="s">
@@ -20060,7 +20099,7 @@
         <v>868</v>
       </c>
       <c r="F250" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D250)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G250" s="3" t="s">
@@ -20096,7 +20135,7 @@
         <v>402</v>
       </c>
       <c r="F251" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D251)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G251" s="3" t="s">
@@ -20132,7 +20171,7 @@
         <v>868</v>
       </c>
       <c r="F252" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D252)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G252" s="3" t="s">
@@ -20168,7 +20207,7 @@
         <v>867</v>
       </c>
       <c r="F253" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D253)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G253" s="3" t="s">
@@ -20204,7 +20243,7 @@
         <v>703</v>
       </c>
       <c r="F254" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D254)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G254" s="3" t="s">
@@ -20240,7 +20279,7 @@
         <v>867</v>
       </c>
       <c r="F255" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D255)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G255" s="3" t="s">
@@ -20276,7 +20315,7 @@
         <v>867</v>
       </c>
       <c r="F256" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D256)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Oui</v>
       </c>
       <c r="G256" s="3" t="s">
@@ -20312,7 +20351,7 @@
         <v>399</v>
       </c>
       <c r="F257" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D257)=1,"Oui","Non")</f>
+        <f t="shared" si="3"/>
         <v>Non</v>
       </c>
       <c r="G257" s="3" t="s">
@@ -20348,7 +20387,7 @@
         <v>867</v>
       </c>
       <c r="F258" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D258)=1,"Oui","Non")</f>
+        <f t="shared" ref="F258:F321" si="4">IF(COUNTIF(D:D,"="&amp;D258)=1,"Oui","Non")</f>
         <v>Oui</v>
       </c>
       <c r="G258" s="3" t="s">
@@ -20384,7 +20423,7 @@
         <v>422</v>
       </c>
       <c r="F259" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D259)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
       <c r="G259" s="3" t="s">
@@ -20420,7 +20459,7 @@
         <v>867</v>
       </c>
       <c r="F260" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D260)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
       <c r="G260" s="3" t="s">
@@ -20456,7 +20495,7 @@
         <v>867</v>
       </c>
       <c r="F261" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D261)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
       <c r="G261" s="3" t="s">
@@ -20492,7 +20531,7 @@
         <v>867</v>
       </c>
       <c r="F262" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D262)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
       <c r="G262" s="3" t="s">
@@ -20528,7 +20567,7 @@
         <v>452</v>
       </c>
       <c r="F263" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D263)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G263" s="3" t="s">
@@ -20564,7 +20603,7 @@
         <v>311</v>
       </c>
       <c r="F264" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D264)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G264" s="3" t="s">
@@ -20583,7 +20622,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>162</v>
       </c>
@@ -20597,11 +20636,26 @@
         <v>245</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>422</v>
+        <v>873</v>
       </c>
       <c r="F265" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D265)=1,"Oui","Non")</f>
-        <v>Oui</v>
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="G265" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="H265" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="I265" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="J265" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="K265" s="3" t="s">
+        <v>872</v>
       </c>
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.25">
@@ -20621,7 +20675,7 @@
         <v>389</v>
       </c>
       <c r="F266" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D266)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G266" s="3" t="s">
@@ -20654,14 +20708,29 @@
         <v>246</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>422</v>
+        <v>873</v>
       </c>
       <c r="F267" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D267)=1,"Oui","Non")</f>
-        <v>Oui</v>
-      </c>
-    </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="G267" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="H267" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="I267" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="J267" s="9">
+        <v>6</v>
+      </c>
+      <c r="K267" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>162</v>
       </c>
@@ -20675,11 +20744,26 @@
         <v>247</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>422</v>
+        <v>877</v>
       </c>
       <c r="F268" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D268)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
+      </c>
+      <c r="G268" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="H268" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="I268" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="J268" s="9">
+        <v>7</v>
+      </c>
+      <c r="K268" s="3" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.25">
@@ -20699,8 +20783,23 @@
         <v>422</v>
       </c>
       <c r="F269" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D269)=1,"Oui","Non")</f>
-        <v>Oui</v>
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="G269" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="H269" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="I269" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="J269" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="K269" s="3" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="270" spans="1:11" x14ac:dyDescent="0.25">
@@ -20717,14 +20816,29 @@
         <v>249</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>422</v>
+        <v>873</v>
       </c>
       <c r="F270" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D270)=1,"Oui","Non")</f>
-        <v>Oui</v>
-      </c>
-    </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="G270" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="H270" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="I270" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="J270" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="K270" s="3" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>162</v>
       </c>
@@ -20738,14 +20852,29 @@
         <v>250</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>422</v>
+        <v>877</v>
       </c>
       <c r="F271" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D271)=1,"Oui","Non")</f>
-        <v>Oui</v>
-      </c>
-    </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="G271" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="H271" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="I271" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="J271" s="9">
+        <v>7</v>
+      </c>
+      <c r="K271" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>162</v>
       </c>
@@ -20759,14 +20888,29 @@
         <v>251</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>422</v>
+        <v>873</v>
       </c>
       <c r="F272" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D272)=1,"Oui","Non")</f>
-        <v>Oui</v>
-      </c>
-    </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="G272" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="H272" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="I272" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="J272" s="9">
+        <v>8</v>
+      </c>
+      <c r="K272" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>162</v>
       </c>
@@ -20783,8 +20927,23 @@
         <v>422</v>
       </c>
       <c r="F273" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D273)=1,"Oui","Non")</f>
-        <v>Oui</v>
+        <f t="shared" si="4"/>
+        <v>Oui</v>
+      </c>
+      <c r="G273" s="3" t="s">
+        <v>884</v>
+      </c>
+      <c r="H273" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="I273" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="J273" s="9">
+        <v>8</v>
+      </c>
+      <c r="K273" s="3" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="274" spans="1:11" x14ac:dyDescent="0.25">
@@ -20804,7 +20963,7 @@
         <v>422</v>
       </c>
       <c r="F274" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D274)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -20825,7 +20984,7 @@
         <v>402</v>
       </c>
       <c r="F275" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D275)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G275" s="3" t="s">
@@ -20861,7 +21020,7 @@
         <v>422</v>
       </c>
       <c r="F276" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D276)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -20882,7 +21041,7 @@
         <v>422</v>
       </c>
       <c r="F277" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D277)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G277" s="3" t="s">
@@ -20918,7 +21077,7 @@
         <v>422</v>
       </c>
       <c r="F278" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D278)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G278" s="3" t="s">
@@ -20954,7 +21113,7 @@
         <v>422</v>
       </c>
       <c r="F279" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D279)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -20975,7 +21134,7 @@
         <v>422</v>
       </c>
       <c r="F280" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D280)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -20996,7 +21155,7 @@
         <v>422</v>
       </c>
       <c r="F281" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D281)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21017,7 +21176,7 @@
         <v>422</v>
       </c>
       <c r="F282" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D282)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21038,7 +21197,7 @@
         <v>422</v>
       </c>
       <c r="F283" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D283)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21059,7 +21218,7 @@
         <v>422</v>
       </c>
       <c r="F284" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D284)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21080,7 +21239,7 @@
         <v>412</v>
       </c>
       <c r="F285" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D285)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G285" s="3" t="s">
@@ -21116,7 +21275,7 @@
         <v>412</v>
       </c>
       <c r="F286" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D286)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G286" s="3" t="s">
@@ -21152,7 +21311,7 @@
         <v>422</v>
       </c>
       <c r="F287" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D287)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21173,7 +21332,7 @@
         <v>422</v>
       </c>
       <c r="F288" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D288)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21194,7 +21353,7 @@
         <v>422</v>
       </c>
       <c r="F289" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D289)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21215,7 +21374,7 @@
         <v>402</v>
       </c>
       <c r="F290" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D290)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G290" s="3" t="s">
@@ -21251,7 +21410,7 @@
         <v>422</v>
       </c>
       <c r="F291" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D291)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21272,7 +21431,7 @@
         <v>573</v>
       </c>
       <c r="F292" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D292)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G292" s="3" t="s">
@@ -21308,7 +21467,7 @@
         <v>422</v>
       </c>
       <c r="F293" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D293)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21329,7 +21488,7 @@
         <v>422</v>
       </c>
       <c r="F294" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D294)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21350,7 +21509,7 @@
         <v>422</v>
       </c>
       <c r="F295" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D295)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21371,7 +21530,7 @@
         <v>422</v>
       </c>
       <c r="F296" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D296)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21392,7 +21551,7 @@
         <v>422</v>
       </c>
       <c r="F297" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D297)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21413,7 +21572,7 @@
         <v>422</v>
       </c>
       <c r="F298" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D298)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21434,7 +21593,7 @@
         <v>425</v>
       </c>
       <c r="F299" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D299)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G299" s="3" t="s">
@@ -21470,7 +21629,7 @@
         <v>402</v>
       </c>
       <c r="F300" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D300)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G300" s="3" t="s">
@@ -21506,7 +21665,7 @@
         <v>422</v>
       </c>
       <c r="F301" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D301)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21527,7 +21686,7 @@
         <v>422</v>
       </c>
       <c r="F302" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D302)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21548,7 +21707,7 @@
         <v>422</v>
       </c>
       <c r="F303" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D303)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21569,7 +21728,7 @@
         <v>422</v>
       </c>
       <c r="F304" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D304)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21590,7 +21749,7 @@
         <v>427</v>
       </c>
       <c r="F305" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D305)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G305" s="3" t="s">
@@ -21626,7 +21785,7 @@
         <v>422</v>
       </c>
       <c r="F306" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D306)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21647,7 +21806,7 @@
         <v>422</v>
       </c>
       <c r="F307" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D307)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21668,7 +21827,7 @@
         <v>422</v>
       </c>
       <c r="F308" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D308)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21689,7 +21848,7 @@
         <v>422</v>
       </c>
       <c r="F309" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D309)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G309" s="3" t="s">
@@ -21725,7 +21884,7 @@
         <v>422</v>
       </c>
       <c r="F310" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D310)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21746,7 +21905,7 @@
         <v>573</v>
       </c>
       <c r="F311" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D311)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G311" s="3" t="s">
@@ -21782,7 +21941,7 @@
         <v>422</v>
       </c>
       <c r="F312" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D312)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21803,7 +21962,7 @@
         <v>422</v>
       </c>
       <c r="F313" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D313)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21824,7 +21983,7 @@
         <v>311</v>
       </c>
       <c r="F314" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D314)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Non</v>
       </c>
       <c r="G314" s="3" t="s">
@@ -21860,7 +22019,7 @@
         <v>422</v>
       </c>
       <c r="F315" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D315)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21881,7 +22040,7 @@
         <v>422</v>
       </c>
       <c r="F316" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D316)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21902,7 +22061,7 @@
         <v>422</v>
       </c>
       <c r="F317" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D317)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21923,7 +22082,7 @@
         <v>422</v>
       </c>
       <c r="F318" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D318)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21944,7 +22103,7 @@
         <v>422</v>
       </c>
       <c r="F319" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D319)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21965,7 +22124,7 @@
         <v>422</v>
       </c>
       <c r="F320" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D320)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -21986,7 +22145,7 @@
         <v>422</v>
       </c>
       <c r="F321" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D321)=1,"Oui","Non")</f>
+        <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22007,7 +22166,7 @@
         <v>422</v>
       </c>
       <c r="F322" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D322)=1,"Oui","Non")</f>
+        <f t="shared" ref="F322:F385" si="5">IF(COUNTIF(D:D,"="&amp;D322)=1,"Oui","Non")</f>
         <v>Oui</v>
       </c>
     </row>
@@ -22028,7 +22187,7 @@
         <v>305</v>
       </c>
       <c r="F323" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D323)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22049,7 +22208,7 @@
         <v>296</v>
       </c>
       <c r="F324" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D324)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22070,7 +22229,7 @@
         <v>296</v>
       </c>
       <c r="F325" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D325)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22091,7 +22250,7 @@
         <v>687</v>
       </c>
       <c r="F326" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D326)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G326" s="3" t="s">
@@ -22127,7 +22286,7 @@
         <v>296</v>
       </c>
       <c r="F327" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D327)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22148,7 +22307,7 @@
         <v>296</v>
       </c>
       <c r="F328" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D328)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22169,7 +22328,7 @@
         <v>296</v>
       </c>
       <c r="F329" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D329)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G329" s="3" t="s">
@@ -22205,7 +22364,7 @@
         <v>422</v>
       </c>
       <c r="F330" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D330)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22226,7 +22385,7 @@
         <v>305</v>
       </c>
       <c r="F331" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D331)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22247,7 +22406,7 @@
         <v>296</v>
       </c>
       <c r="F332" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D332)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22268,7 +22427,7 @@
         <v>296</v>
       </c>
       <c r="F333" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D333)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22289,7 +22448,7 @@
         <v>422</v>
       </c>
       <c r="F334" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D334)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22310,7 +22469,7 @@
         <v>311</v>
       </c>
       <c r="F335" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D335)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G335" s="3" t="s">
@@ -22346,7 +22505,7 @@
         <v>422</v>
       </c>
       <c r="F336" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D336)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22367,7 +22526,7 @@
         <v>422</v>
       </c>
       <c r="F337" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D337)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22388,7 +22547,7 @@
         <v>422</v>
       </c>
       <c r="F338" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D338)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22409,7 +22568,7 @@
         <v>407</v>
       </c>
       <c r="F339" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D339)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G339" s="3" t="s">
@@ -22445,7 +22604,7 @@
         <v>296</v>
       </c>
       <c r="F340" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D340)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22466,7 +22625,7 @@
         <v>296</v>
       </c>
       <c r="F341" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D341)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22487,7 +22646,7 @@
         <v>422</v>
       </c>
       <c r="F342" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D342)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22508,7 +22667,7 @@
         <v>316</v>
       </c>
       <c r="F343" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D343)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22529,7 +22688,7 @@
         <v>422</v>
       </c>
       <c r="F344" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D344)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22550,7 +22709,7 @@
         <v>422</v>
       </c>
       <c r="F345" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D345)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22571,7 +22730,7 @@
         <v>422</v>
       </c>
       <c r="F346" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D346)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22592,7 +22751,7 @@
         <v>389</v>
       </c>
       <c r="F347" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D347)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G347" s="3" t="s">
@@ -22628,7 +22787,7 @@
         <v>422</v>
       </c>
       <c r="F348" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D348)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22649,7 +22808,7 @@
         <v>422</v>
       </c>
       <c r="F349" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D349)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22670,7 +22829,7 @@
         <v>422</v>
       </c>
       <c r="F350" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D350)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22691,7 +22850,7 @@
         <v>427</v>
       </c>
       <c r="F351" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D351)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G351" s="3" t="s">
@@ -22727,7 +22886,7 @@
         <v>422</v>
       </c>
       <c r="F352" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D352)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22748,7 +22907,7 @@
         <v>422</v>
       </c>
       <c r="F353" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D353)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22769,7 +22928,7 @@
         <v>422</v>
       </c>
       <c r="F354" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D354)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22790,7 +22949,7 @@
         <v>422</v>
       </c>
       <c r="F355" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D355)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22811,7 +22970,7 @@
         <v>399</v>
       </c>
       <c r="F356" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D356)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G356" s="3" t="s">
@@ -22847,7 +23006,7 @@
         <v>422</v>
       </c>
       <c r="F357" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D357)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22868,7 +23027,7 @@
         <v>422</v>
       </c>
       <c r="F358" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D358)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22889,7 +23048,7 @@
         <v>422</v>
       </c>
       <c r="F359" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D359)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22910,7 +23069,7 @@
         <v>407</v>
       </c>
       <c r="F360" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D360)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G360" s="3" t="s">
@@ -22946,7 +23105,7 @@
         <v>422</v>
       </c>
       <c r="F361" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D361)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22967,7 +23126,7 @@
         <v>316</v>
       </c>
       <c r="F362" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D362)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -22988,7 +23147,7 @@
         <v>422</v>
       </c>
       <c r="F363" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D363)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23009,7 +23168,7 @@
         <v>422</v>
       </c>
       <c r="F364" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D364)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23030,7 +23189,7 @@
         <v>422</v>
       </c>
       <c r="F365" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D365)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23051,7 +23210,7 @@
         <v>422</v>
       </c>
       <c r="F366" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D366)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23072,7 +23231,7 @@
         <v>422</v>
       </c>
       <c r="F367" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D367)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23093,7 +23252,7 @@
         <v>389</v>
       </c>
       <c r="F368" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D368)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G368" s="3" t="s">
@@ -23129,7 +23288,7 @@
         <v>422</v>
       </c>
       <c r="F369" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D369)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23150,7 +23309,7 @@
         <v>422</v>
       </c>
       <c r="F370" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D370)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23171,7 +23330,7 @@
         <v>422</v>
       </c>
       <c r="F371" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D371)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23192,7 +23351,7 @@
         <v>422</v>
       </c>
       <c r="F372" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D372)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G372" s="3" t="s">
@@ -23228,7 +23387,7 @@
         <v>422</v>
       </c>
       <c r="F373" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D373)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23249,7 +23408,7 @@
         <v>422</v>
       </c>
       <c r="F374" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D374)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23270,7 +23429,7 @@
         <v>422</v>
       </c>
       <c r="F375" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D375)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23291,7 +23450,7 @@
         <v>422</v>
       </c>
       <c r="F376" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D376)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23312,7 +23471,7 @@
         <v>422</v>
       </c>
       <c r="F377" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D377)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23333,7 +23492,7 @@
         <v>422</v>
       </c>
       <c r="F378" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D378)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23354,7 +23513,7 @@
         <v>422</v>
       </c>
       <c r="F379" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D379)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23375,7 +23534,7 @@
         <v>628</v>
       </c>
       <c r="F380" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D380)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G380" s="3" t="s">
@@ -23411,7 +23570,7 @@
         <v>422</v>
       </c>
       <c r="F381" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D381)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23432,7 +23591,7 @@
         <v>298</v>
       </c>
       <c r="F382" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D382)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
     </row>
@@ -23453,7 +23612,7 @@
         <v>520</v>
       </c>
       <c r="F383" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D383)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
       <c r="G383" s="3" t="s">
@@ -23489,7 +23648,7 @@
         <v>407</v>
       </c>
       <c r="F384" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D384)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Non</v>
       </c>
       <c r="G384" s="3" t="s">
@@ -23525,7 +23684,7 @@
         <v>422</v>
       </c>
       <c r="F385" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D385)=1,"Oui","Non")</f>
+        <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
       <c r="G385" s="3" t="s">
@@ -23561,7 +23720,7 @@
         <v>412</v>
       </c>
       <c r="F386" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D386)=1,"Oui","Non")</f>
+        <f t="shared" ref="F386:F422" si="6">IF(COUNTIF(D:D,"="&amp;D386)=1,"Oui","Non")</f>
         <v>Oui</v>
       </c>
       <c r="G386" s="3" t="s">
@@ -23597,7 +23756,7 @@
         <v>412</v>
       </c>
       <c r="F387" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D387)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Non</v>
       </c>
       <c r="G387" s="3" t="s">
@@ -23633,7 +23792,7 @@
         <v>628</v>
       </c>
       <c r="F388" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D388)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G388" s="3" t="s">
@@ -23669,7 +23828,7 @@
         <v>520</v>
       </c>
       <c r="F389" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D389)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G389" s="3" t="s">
@@ -23705,7 +23864,7 @@
         <v>520</v>
       </c>
       <c r="F390" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D390)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G390" s="3" t="s">
@@ -23741,7 +23900,7 @@
         <v>633</v>
       </c>
       <c r="F391" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D391)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G391" s="3" t="s">
@@ -23777,7 +23936,7 @@
         <v>592</v>
       </c>
       <c r="F392" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D392)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G392" s="3" t="s">
@@ -23813,7 +23972,7 @@
         <v>633</v>
       </c>
       <c r="F393" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D393)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G393" s="3" t="s">
@@ -23849,7 +24008,7 @@
         <v>633</v>
       </c>
       <c r="F394" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D394)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G394" s="3" t="s">
@@ -23885,7 +24044,7 @@
         <v>412</v>
       </c>
       <c r="F395" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D395)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G395" s="3" t="s">
@@ -23921,7 +24080,7 @@
         <v>427</v>
       </c>
       <c r="F396" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D396)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G396" s="3" t="s">
@@ -23957,7 +24116,7 @@
         <v>422</v>
       </c>
       <c r="F397" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D397)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G397" s="3" t="s">
@@ -23993,7 +24152,7 @@
         <v>646</v>
       </c>
       <c r="F398" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D398)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G398" s="3" t="s">
@@ -24029,7 +24188,7 @@
         <v>628</v>
       </c>
       <c r="F399" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D399)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Non</v>
       </c>
       <c r="G399" s="3" t="s">
@@ -24065,7 +24224,7 @@
         <v>311</v>
       </c>
       <c r="F400" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D400)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G400" s="3" t="s">
@@ -24101,7 +24260,7 @@
         <v>633</v>
       </c>
       <c r="F401" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D401)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Non</v>
       </c>
       <c r="G401" s="3" t="s">
@@ -24137,7 +24296,7 @@
         <v>628</v>
       </c>
       <c r="F402" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D402)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G402" s="3" t="s">
@@ -24173,7 +24332,7 @@
         <v>653</v>
       </c>
       <c r="F403" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D403)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G403" s="3" t="s">
@@ -24209,7 +24368,7 @@
         <v>676</v>
       </c>
       <c r="F404" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D404)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G404" s="3" t="s">
@@ -24245,7 +24404,7 @@
         <v>427</v>
       </c>
       <c r="F405" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D405)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G405" s="3" t="s">
@@ -24281,7 +24440,7 @@
         <v>633</v>
       </c>
       <c r="F406" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D406)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G406" s="3" t="s">
@@ -24317,7 +24476,7 @@
         <v>389</v>
       </c>
       <c r="F407" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D407)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Non</v>
       </c>
       <c r="G407" s="3" t="s">
@@ -24350,10 +24509,10 @@
         <v>247</v>
       </c>
       <c r="E408" s="1" t="s">
-        <v>422</v>
+        <v>877</v>
       </c>
       <c r="F408" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D408)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Non</v>
       </c>
     </row>
@@ -24374,7 +24533,7 @@
         <v>520</v>
       </c>
       <c r="F409" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D409)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G409" s="3" t="s">
@@ -24410,7 +24569,7 @@
         <v>673</v>
       </c>
       <c r="F410" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D410)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G410" s="3" t="s">
@@ -24446,7 +24605,7 @@
         <v>653</v>
       </c>
       <c r="F411" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D411)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G411" s="3" t="s">
@@ -24482,7 +24641,7 @@
         <v>769</v>
       </c>
       <c r="F412" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D412)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Non</v>
       </c>
       <c r="G412" s="3" t="s">
@@ -24518,7 +24677,7 @@
         <v>422</v>
       </c>
       <c r="F413" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D413)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G413" s="3" t="s">
@@ -24554,7 +24713,7 @@
         <v>676</v>
       </c>
       <c r="F414" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D414)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G414" s="3" t="s">
@@ -24590,7 +24749,7 @@
         <v>439</v>
       </c>
       <c r="F415" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D415)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Non</v>
       </c>
       <c r="G415" s="3" t="s">
@@ -24626,7 +24785,7 @@
         <v>653</v>
       </c>
       <c r="F416" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D416)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G416" s="3" t="s">
@@ -24662,7 +24821,7 @@
         <v>676</v>
       </c>
       <c r="F417" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D417)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G417" s="3" t="s">
@@ -24698,7 +24857,7 @@
         <v>422</v>
       </c>
       <c r="F418" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D418)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Non</v>
       </c>
       <c r="G418" s="3" t="s">
@@ -24734,7 +24893,7 @@
         <v>653</v>
       </c>
       <c r="F419" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D419)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G419" s="3" t="s">
@@ -24770,7 +24929,7 @@
         <v>422</v>
       </c>
       <c r="F420" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D420)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Non</v>
       </c>
       <c r="G420" s="3" t="s">
@@ -24806,7 +24965,7 @@
         <v>673</v>
       </c>
       <c r="F421" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D421)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G421" s="3" t="s">
@@ -24842,7 +25001,7 @@
         <v>653</v>
       </c>
       <c r="F422" s="1" t="str">
-        <f>IF(COUNTIF(D:D,"="&amp;D422)=1,"Oui","Non")</f>
+        <f t="shared" si="6"/>
         <v>Oui</v>
       </c>
       <c r="G422" s="3" t="s">
@@ -24879,7 +25038,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25097,10 +25256,13 @@
         <v>244</v>
       </c>
       <c r="C15" t="s">
+        <v>874</v>
+      </c>
+      <c r="D15" t="s">
+        <v>873</v>
+      </c>
+      <c r="E15" t="s">
         <v>870</v>
-      </c>
-      <c r="E15" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fils de Fenrir finis
</commit_message>
<xml_diff>
--- a/Liste de dons LG Apocalypse.xlsx
+++ b/Liste de dons LG Apocalypse.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{414E4CC9-A408-4207-968D-236C41C2FC72}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091FD884-DF49-4266-831F-39E42F629FD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Repartition thèmes par liste" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Dons d''origine'!$A$1:$K$422</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Listes par type'!$A$1:$D$22</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
@@ -24,12 +24,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3406" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3432" uniqueCount="895">
   <si>
     <t>Liste</t>
   </si>
@@ -2692,6 +2698,36 @@
   </si>
   <si>
     <t>Redirige la douleur de ses blessures à ceux qui les lui ont infligées</t>
+  </si>
+  <si>
+    <t>Change le sang du LG en bile qui empoisonne au contact</t>
+  </si>
+  <si>
+    <t>Le LG ne peut plus échouer un test de Vigueur</t>
+  </si>
+  <si>
+    <t>1 V + 1 R</t>
+  </si>
+  <si>
+    <t>Double la Vigueur du LG</t>
+  </si>
+  <si>
+    <t>Invoque des grands loups pour l'aider</t>
+  </si>
+  <si>
+    <t>Rage et Gnose variable</t>
+  </si>
+  <si>
+    <t>La morsure du LG peut estropier les membres</t>
+  </si>
+  <si>
+    <t>Force + Insctinct primal</t>
+  </si>
+  <si>
+    <t>Invoque un Avatar du Grand Fenrir</t>
+  </si>
+  <si>
+    <t>Vigueur + Occultisme</t>
   </si>
 </sst>
 </file>
@@ -2812,7 +2848,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Auteur" refreshedDate="43643.43254386574" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="420" xr:uid="{2C21D036-61B9-4234-91DA-1EFDCFF6F2F1}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Autor" refreshedDate="43643.43254386574" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="420" xr:uid="{2C21D036-61B9-4234-91DA-1EFDCFF6F2F1}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:K422" sheet="Dons d'origine"/>
   </cacheSource>
@@ -9049,36 +9085,36 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.86328125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>559</v>
       </c>
@@ -9086,7 +9122,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>161</v>
       </c>
@@ -9100,7 +9136,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>835</v>
       </c>
@@ -9168,7 +9204,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>422</v>
       </c>
@@ -9235,7 +9271,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>770</v>
       </c>
@@ -9266,7 +9302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>520</v>
       </c>
@@ -9305,7 +9341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>305</v>
       </c>
@@ -9340,7 +9376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>802</v>
       </c>
@@ -9371,7 +9407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>452</v>
       </c>
@@ -9406,7 +9442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>768</v>
       </c>
@@ -9437,7 +9473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>676</v>
       </c>
@@ -9468,7 +9504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>703</v>
       </c>
@@ -9501,7 +9537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>573</v>
       </c>
@@ -9538,7 +9574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>783</v>
       </c>
@@ -9573,7 +9609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>687</v>
       </c>
@@ -9610,7 +9646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>298</v>
       </c>
@@ -9645,7 +9681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>311</v>
       </c>
@@ -9692,7 +9728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>646</v>
       </c>
@@ -9723,7 +9759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>628</v>
       </c>
@@ -9756,7 +9792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>594</v>
       </c>
@@ -9791,7 +9827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>93</v>
       </c>
@@ -9824,7 +9860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>415</v>
       </c>
@@ -9855,7 +9891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>817</v>
       </c>
@@ -9886,7 +9922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>427</v>
       </c>
@@ -9931,7 +9967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>222</v>
       </c>
@@ -9966,7 +10002,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>821</v>
       </c>
@@ -9997,7 +10033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>797</v>
       </c>
@@ -10030,7 +10066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>653</v>
       </c>
@@ -10061,7 +10097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>560</v>
       </c>
@@ -10094,7 +10130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>633</v>
       </c>
@@ -10131,7 +10167,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>804</v>
       </c>
@@ -10162,7 +10198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>595</v>
       </c>
@@ -10201,7 +10237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>402</v>
       </c>
@@ -10248,7 +10284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>673</v>
       </c>
@@ -10279,7 +10315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>757</v>
       </c>
@@ -10312,7 +10348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>425</v>
       </c>
@@ -10347,7 +10383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>824</v>
       </c>
@@ -10378,7 +10414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>412</v>
       </c>
@@ -10429,7 +10465,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>678</v>
       </c>
@@ -10460,7 +10496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>496</v>
       </c>
@@ -10493,7 +10529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A43" s="6" t="s">
         <v>389</v>
       </c>
@@ -10542,7 +10578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A44" s="6" t="s">
         <v>712</v>
       </c>
@@ -10573,7 +10609,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A45" s="6" t="s">
         <v>769</v>
       </c>
@@ -10606,7 +10642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A46" s="6" t="s">
         <v>439</v>
       </c>
@@ -10639,7 +10675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A47" s="6" t="s">
         <v>407</v>
       </c>
@@ -10682,7 +10718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A48" s="6" t="s">
         <v>395</v>
       </c>
@@ -10717,7 +10753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A49" s="6" t="s">
         <v>592</v>
       </c>
@@ -10750,7 +10786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A50" s="6" t="s">
         <v>316</v>
       </c>
@@ -10783,7 +10819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A51" s="6" t="s">
         <v>296</v>
       </c>
@@ -10820,7 +10856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A52" s="6" t="s">
         <v>399</v>
       </c>
@@ -10857,7 +10893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A53" s="6" t="s">
         <v>491</v>
       </c>
@@ -10888,7 +10924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A54" s="6" t="s">
         <v>488</v>
       </c>
@@ -10923,7 +10959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A55" s="6" t="s">
         <v>576</v>
       </c>
@@ -10960,7 +10996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A56" s="6" t="s">
         <v>652</v>
       </c>
@@ -10995,7 +11031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A57" s="6" t="s">
         <v>836</v>
       </c>
@@ -11026,7 +11062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A58" s="6" t="s">
         <v>834</v>
       </c>
@@ -11108,27 +11144,27 @@
   <dimension ref="A1:K422"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E274" sqref="E274"/>
+      <pane ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A282" sqref="A282"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.86328125" style="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="31" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>159</v>
       </c>
@@ -11163,7 +11199,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>160</v>
       </c>
@@ -11199,7 +11235,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>160</v>
       </c>
@@ -11235,7 +11271,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>160</v>
       </c>
@@ -11271,7 +11307,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>160</v>
       </c>
@@ -11307,7 +11343,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
@@ -11343,7 +11379,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>160</v>
       </c>
@@ -11379,7 +11415,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>160</v>
       </c>
@@ -11415,7 +11451,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>160</v>
       </c>
@@ -11451,7 +11487,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>160</v>
       </c>
@@ -11487,7 +11523,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>160</v>
       </c>
@@ -11523,7 +11559,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>160</v>
       </c>
@@ -11559,7 +11595,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>160</v>
       </c>
@@ -11595,7 +11631,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>160</v>
       </c>
@@ -11631,7 +11667,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>160</v>
       </c>
@@ -11667,7 +11703,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>160</v>
       </c>
@@ -11703,7 +11739,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>160</v>
       </c>
@@ -11739,7 +11775,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>160</v>
       </c>
@@ -11775,7 +11811,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>160</v>
       </c>
@@ -11811,7 +11847,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>160</v>
       </c>
@@ -11847,7 +11883,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>160</v>
       </c>
@@ -11883,7 +11919,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>160</v>
       </c>
@@ -11919,7 +11955,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>160</v>
       </c>
@@ -11955,7 +11991,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>160</v>
       </c>
@@ -11991,7 +12027,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>160</v>
       </c>
@@ -12027,7 +12063,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>160</v>
       </c>
@@ -12063,7 +12099,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>160</v>
       </c>
@@ -12096,7 +12132,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>160</v>
       </c>
@@ -12132,7 +12168,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>160</v>
       </c>
@@ -12165,7 +12201,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>160</v>
       </c>
@@ -12201,7 +12237,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>160</v>
       </c>
@@ -12237,7 +12273,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>160</v>
       </c>
@@ -12273,7 +12309,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>160</v>
       </c>
@@ -12309,7 +12345,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>160</v>
       </c>
@@ -12345,7 +12381,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>160</v>
       </c>
@@ -12381,7 +12417,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>160</v>
       </c>
@@ -12417,7 +12453,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>160</v>
       </c>
@@ -12453,7 +12489,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>160</v>
       </c>
@@ -12489,7 +12525,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>160</v>
       </c>
@@ -12525,7 +12561,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>160</v>
       </c>
@@ -12561,7 +12597,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>160</v>
       </c>
@@ -12597,7 +12633,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>160</v>
       </c>
@@ -12633,7 +12669,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>160</v>
       </c>
@@ -12669,7 +12705,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>160</v>
       </c>
@@ -12705,7 +12741,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>160</v>
       </c>
@@ -12741,7 +12777,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>160</v>
       </c>
@@ -12777,7 +12813,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>160</v>
       </c>
@@ -12813,7 +12849,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>160</v>
       </c>
@@ -12849,7 +12885,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>160</v>
       </c>
@@ -12885,7 +12921,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>160</v>
       </c>
@@ -12921,7 +12957,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>160</v>
       </c>
@@ -12957,7 +12993,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>160</v>
       </c>
@@ -12993,7 +13029,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>160</v>
       </c>
@@ -13029,7 +13065,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>160</v>
       </c>
@@ -13065,7 +13101,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>160</v>
       </c>
@@ -13101,7 +13137,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>160</v>
       </c>
@@ -13137,7 +13173,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>160</v>
       </c>
@@ -13173,7 +13209,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>160</v>
       </c>
@@ -13209,7 +13245,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>160</v>
       </c>
@@ -13245,7 +13281,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>160</v>
       </c>
@@ -13281,7 +13317,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>160</v>
       </c>
@@ -13317,7 +13353,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>161</v>
       </c>
@@ -13353,7 +13389,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>161</v>
       </c>
@@ -13389,7 +13425,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>161</v>
       </c>
@@ -13425,7 +13461,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>161</v>
       </c>
@@ -13461,7 +13497,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>161</v>
       </c>
@@ -13497,7 +13533,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>161</v>
       </c>
@@ -13533,7 +13569,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>161</v>
       </c>
@@ -13569,7 +13605,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>161</v>
       </c>
@@ -13605,7 +13641,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>161</v>
       </c>
@@ -13641,7 +13677,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>161</v>
       </c>
@@ -13677,7 +13713,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>161</v>
       </c>
@@ -13713,7 +13749,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>161</v>
       </c>
@@ -13749,7 +13785,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>161</v>
       </c>
@@ -13785,7 +13821,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>161</v>
       </c>
@@ -13821,7 +13857,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
         <v>161</v>
       </c>
@@ -13857,7 +13893,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
         <v>161</v>
       </c>
@@ -13893,7 +13929,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>161</v>
       </c>
@@ -13929,7 +13965,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>161</v>
       </c>
@@ -13965,7 +14001,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
         <v>161</v>
       </c>
@@ -14001,7 +14037,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="2" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>161</v>
       </c>
@@ -14037,7 +14073,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>161</v>
       </c>
@@ -14073,7 +14109,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>161</v>
       </c>
@@ -14109,7 +14145,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
         <v>161</v>
       </c>
@@ -14145,7 +14181,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>161</v>
       </c>
@@ -14181,7 +14217,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>161</v>
       </c>
@@ -14217,7 +14253,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>161</v>
       </c>
@@ -14253,7 +14289,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>161</v>
       </c>
@@ -14289,7 +14325,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>161</v>
       </c>
@@ -14325,7 +14361,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
         <v>161</v>
       </c>
@@ -14361,7 +14397,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
         <v>161</v>
       </c>
@@ -14397,7 +14433,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>161</v>
       </c>
@@ -14433,7 +14469,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>161</v>
       </c>
@@ -14469,7 +14505,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>161</v>
       </c>
@@ -14505,7 +14541,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>161</v>
       </c>
@@ -14541,7 +14577,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
         <v>161</v>
       </c>
@@ -14577,7 +14613,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
         <v>161</v>
       </c>
@@ -14613,7 +14649,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
         <v>161</v>
       </c>
@@ -14649,7 +14685,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
         <v>161</v>
       </c>
@@ -14685,7 +14721,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
         <v>161</v>
       </c>
@@ -14721,7 +14757,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>161</v>
       </c>
@@ -14757,7 +14793,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="102" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A102" s="2" t="s">
         <v>161</v>
       </c>
@@ -14793,7 +14829,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
         <v>161</v>
       </c>
@@ -14829,7 +14865,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
         <v>161</v>
       </c>
@@ -14865,7 +14901,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
         <v>161</v>
       </c>
@@ -14901,7 +14937,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>161</v>
       </c>
@@ -14937,7 +14973,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>161</v>
       </c>
@@ -14973,7 +15009,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
         <v>161</v>
       </c>
@@ -15009,7 +15045,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
         <v>161</v>
       </c>
@@ -15045,7 +15081,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
         <v>161</v>
       </c>
@@ -15081,7 +15117,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
         <v>161</v>
       </c>
@@ -15117,7 +15153,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
         <v>161</v>
       </c>
@@ -15153,7 +15189,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
         <v>161</v>
       </c>
@@ -15189,7 +15225,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
         <v>161</v>
       </c>
@@ -15225,7 +15261,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
         <v>161</v>
       </c>
@@ -15261,7 +15297,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A116" s="1" t="s">
         <v>161</v>
       </c>
@@ -15297,7 +15333,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
         <v>161</v>
       </c>
@@ -15333,7 +15369,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
         <v>161</v>
       </c>
@@ -15369,7 +15405,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="s">
         <v>161</v>
       </c>
@@ -15402,7 +15438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A120" s="1" t="s">
         <v>161</v>
       </c>
@@ -15438,7 +15474,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A121" s="1" t="s">
         <v>161</v>
       </c>
@@ -15474,7 +15510,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="s">
         <v>161</v>
       </c>
@@ -15510,7 +15546,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A123" s="1" t="s">
         <v>161</v>
       </c>
@@ -15546,7 +15582,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A124" s="1" t="s">
         <v>161</v>
       </c>
@@ -15582,7 +15618,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A125" s="1" t="s">
         <v>161</v>
       </c>
@@ -15618,7 +15654,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A126" s="1" t="s">
         <v>161</v>
       </c>
@@ -15654,7 +15690,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
         <v>161</v>
       </c>
@@ -15690,7 +15726,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A128" s="1" t="s">
         <v>161</v>
       </c>
@@ -15726,7 +15762,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A129" s="1" t="s">
         <v>161</v>
       </c>
@@ -15762,7 +15798,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A130" s="1" t="s">
         <v>161</v>
       </c>
@@ -15798,7 +15834,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A131" s="1" t="s">
         <v>161</v>
       </c>
@@ -15834,7 +15870,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A132" s="1" t="s">
         <v>161</v>
       </c>
@@ -15870,7 +15906,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A133" s="1" t="s">
         <v>161</v>
       </c>
@@ -15906,7 +15942,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A134" s="1" t="s">
         <v>161</v>
       </c>
@@ -15942,7 +15978,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A135" s="1" t="s">
         <v>161</v>
       </c>
@@ -15978,7 +16014,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A136" s="1" t="s">
         <v>161</v>
       </c>
@@ -16014,7 +16050,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A137" s="1" t="s">
         <v>161</v>
       </c>
@@ -16050,7 +16086,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A138" s="1" t="s">
         <v>161</v>
       </c>
@@ -16086,7 +16122,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A139" s="1" t="s">
         <v>161</v>
       </c>
@@ -16122,7 +16158,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A140" s="1" t="s">
         <v>161</v>
       </c>
@@ -16158,7 +16194,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A141" s="1" t="s">
         <v>161</v>
       </c>
@@ -16194,7 +16230,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A142" s="1" t="s">
         <v>161</v>
       </c>
@@ -16230,7 +16266,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A143" s="1" t="s">
         <v>161</v>
       </c>
@@ -16266,7 +16302,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A144" s="1" t="s">
         <v>161</v>
       </c>
@@ -16302,7 +16338,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A145" s="1" t="s">
         <v>161</v>
       </c>
@@ -16338,7 +16374,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A146" s="1" t="s">
         <v>161</v>
       </c>
@@ -16374,7 +16410,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A147" s="1" t="s">
         <v>161</v>
       </c>
@@ -16410,7 +16446,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A148" s="1" t="s">
         <v>161</v>
       </c>
@@ -16446,7 +16482,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A149" s="1" t="s">
         <v>161</v>
       </c>
@@ -16482,7 +16518,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A150" s="1" t="s">
         <v>161</v>
       </c>
@@ -16518,7 +16554,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A151" s="1" t="s">
         <v>161</v>
       </c>
@@ -16554,7 +16590,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A152" s="1" t="s">
         <v>161</v>
       </c>
@@ -16590,7 +16626,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A153" s="1" t="s">
         <v>161</v>
       </c>
@@ -16626,7 +16662,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A154" s="1" t="s">
         <v>161</v>
       </c>
@@ -16662,7 +16698,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A155" s="1" t="s">
         <v>161</v>
       </c>
@@ -16698,7 +16734,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A156" s="1" t="s">
         <v>161</v>
       </c>
@@ -16734,7 +16770,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A157" s="1" t="s">
         <v>161</v>
       </c>
@@ -16770,7 +16806,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A158" s="1" t="s">
         <v>161</v>
       </c>
@@ -16806,7 +16842,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A159" s="1" t="s">
         <v>161</v>
       </c>
@@ -16842,7 +16878,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A160" s="1" t="s">
         <v>161</v>
       </c>
@@ -16878,7 +16914,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A161" s="1" t="s">
         <v>161</v>
       </c>
@@ -16914,7 +16950,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A162" s="1" t="s">
         <v>161</v>
       </c>
@@ -16950,7 +16986,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A163" s="1" t="s">
         <v>162</v>
       </c>
@@ -16986,7 +17022,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
@@ -17022,7 +17058,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A165" s="1" t="s">
         <v>162</v>
       </c>
@@ -17058,7 +17094,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A166" s="1" t="s">
         <v>162</v>
       </c>
@@ -17094,7 +17130,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A167" s="1" t="s">
         <v>162</v>
       </c>
@@ -17130,7 +17166,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A168" s="1" t="s">
         <v>162</v>
       </c>
@@ -17166,7 +17202,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A169" s="1" t="s">
         <v>162</v>
       </c>
@@ -17202,7 +17238,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A170" s="1" t="s">
         <v>162</v>
       </c>
@@ -17238,7 +17274,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="171" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A171" s="2" t="s">
         <v>162</v>
       </c>
@@ -17274,7 +17310,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A172" s="1" t="s">
         <v>162</v>
       </c>
@@ -17310,7 +17346,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A173" s="1" t="s">
         <v>162</v>
       </c>
@@ -17346,7 +17382,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A174" s="1" t="s">
         <v>162</v>
       </c>
@@ -17382,7 +17418,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A175" s="1" t="s">
         <v>162</v>
       </c>
@@ -17418,7 +17454,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A176" s="1" t="s">
         <v>162</v>
       </c>
@@ -17454,7 +17490,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A177" s="1" t="s">
         <v>162</v>
       </c>
@@ -17490,7 +17526,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A178" s="1" t="s">
         <v>162</v>
       </c>
@@ -17526,7 +17562,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A179" s="1" t="s">
         <v>162</v>
       </c>
@@ -17562,7 +17598,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A180" s="1" t="s">
         <v>162</v>
       </c>
@@ -17598,7 +17634,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A181" s="1" t="s">
         <v>162</v>
       </c>
@@ -17634,7 +17670,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A182" s="1" t="s">
         <v>162</v>
       </c>
@@ -17670,7 +17706,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A183" s="1" t="s">
         <v>162</v>
       </c>
@@ -17706,7 +17742,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A184" s="1" t="s">
         <v>162</v>
       </c>
@@ -17742,7 +17778,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A185" s="1" t="s">
         <v>162</v>
       </c>
@@ -17778,7 +17814,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A186" s="1" t="s">
         <v>162</v>
       </c>
@@ -17814,7 +17850,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A187" s="1" t="s">
         <v>162</v>
       </c>
@@ -17850,7 +17886,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A188" s="1" t="s">
         <v>162</v>
       </c>
@@ -17886,7 +17922,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A189" s="1" t="s">
         <v>162</v>
       </c>
@@ -17922,7 +17958,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A190" s="1" t="s">
         <v>162</v>
       </c>
@@ -17958,7 +17994,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A191" s="1" t="s">
         <v>162</v>
       </c>
@@ -17994,7 +18030,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A192" s="1" t="s">
         <v>162</v>
       </c>
@@ -18030,7 +18066,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A193" s="1" t="s">
         <v>162</v>
       </c>
@@ -18066,7 +18102,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A194" s="1" t="s">
         <v>162</v>
       </c>
@@ -18102,7 +18138,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A195" s="1" t="s">
         <v>162</v>
       </c>
@@ -18138,7 +18174,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A196" s="1" t="s">
         <v>162</v>
       </c>
@@ -18174,7 +18210,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A197" s="1" t="s">
         <v>162</v>
       </c>
@@ -18210,7 +18246,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="198" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A198" s="1" t="s">
         <v>162</v>
       </c>
@@ -18246,7 +18282,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A199" s="1" t="s">
         <v>162</v>
       </c>
@@ -18282,7 +18318,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A200" s="1" t="s">
         <v>162</v>
       </c>
@@ -18318,7 +18354,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A201" s="1" t="s">
         <v>162</v>
       </c>
@@ -18354,7 +18390,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="202" spans="1:11" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" s="2" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A202" s="2" t="s">
         <v>162</v>
       </c>
@@ -18390,7 +18426,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A203" s="1" t="s">
         <v>162</v>
       </c>
@@ -18426,7 +18462,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A204" s="1" t="s">
         <v>162</v>
       </c>
@@ -18462,7 +18498,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A205" s="1" t="s">
         <v>162</v>
       </c>
@@ -18498,7 +18534,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A206" s="1" t="s">
         <v>162</v>
       </c>
@@ -18534,7 +18570,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A207" s="1" t="s">
         <v>162</v>
       </c>
@@ -18570,7 +18606,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A208" s="1" t="s">
         <v>162</v>
       </c>
@@ -18606,7 +18642,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="209" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A209" s="1" t="s">
         <v>162</v>
       </c>
@@ -18642,7 +18678,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A210" s="1" t="s">
         <v>162</v>
       </c>
@@ -18678,7 +18714,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A211" s="1" t="s">
         <v>162</v>
       </c>
@@ -18714,7 +18750,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="212" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A212" s="1" t="s">
         <v>162</v>
       </c>
@@ -18750,7 +18786,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="213" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A213" s="1" t="s">
         <v>162</v>
       </c>
@@ -18786,7 +18822,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A214" s="1" t="s">
         <v>162</v>
       </c>
@@ -18822,7 +18858,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A215" s="1" t="s">
         <v>162</v>
       </c>
@@ -18858,7 +18894,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="216" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A216" s="1" t="s">
         <v>162</v>
       </c>
@@ -18894,7 +18930,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A217" s="1" t="s">
         <v>162</v>
       </c>
@@ -18930,7 +18966,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="218" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A218" s="1" t="s">
         <v>162</v>
       </c>
@@ -18966,7 +19002,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A219" s="1" t="s">
         <v>162</v>
       </c>
@@ -19002,7 +19038,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A220" s="1" t="s">
         <v>162</v>
       </c>
@@ -19038,7 +19074,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="221" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A221" s="1" t="s">
         <v>162</v>
       </c>
@@ -19074,7 +19110,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A222" s="1" t="s">
         <v>162</v>
       </c>
@@ -19110,7 +19146,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A223" s="1" t="s">
         <v>162</v>
       </c>
@@ -19146,7 +19182,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="224" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A224" s="1" t="s">
         <v>162</v>
       </c>
@@ -19182,7 +19218,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A225" s="1" t="s">
         <v>162</v>
       </c>
@@ -19218,7 +19254,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A226" s="1" t="s">
         <v>162</v>
       </c>
@@ -19254,7 +19290,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A227" s="1" t="s">
         <v>162</v>
       </c>
@@ -19290,7 +19326,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A228" s="1" t="s">
         <v>162</v>
       </c>
@@ -19326,7 +19362,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="229" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A229" s="1" t="s">
         <v>162</v>
       </c>
@@ -19362,7 +19398,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="230" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A230" s="1" t="s">
         <v>162</v>
       </c>
@@ -19398,7 +19434,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="231" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A231" s="1" t="s">
         <v>162</v>
       </c>
@@ -19434,7 +19470,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A232" s="1" t="s">
         <v>162</v>
       </c>
@@ -19470,7 +19506,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="233" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A233" s="1" t="s">
         <v>162</v>
       </c>
@@ -19506,7 +19542,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A234" s="1" t="s">
         <v>162</v>
       </c>
@@ -19542,7 +19578,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A235" s="1" t="s">
         <v>162</v>
       </c>
@@ -19578,7 +19614,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="236" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A236" s="1" t="s">
         <v>162</v>
       </c>
@@ -19614,7 +19650,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="237" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A237" s="1" t="s">
         <v>162</v>
       </c>
@@ -19650,7 +19686,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="238" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A238" s="1" t="s">
         <v>162</v>
       </c>
@@ -19686,7 +19722,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A239" s="1" t="s">
         <v>162</v>
       </c>
@@ -19722,7 +19758,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A240" s="1" t="s">
         <v>162</v>
       </c>
@@ -19758,7 +19794,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="241" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A241" s="1" t="s">
         <v>162</v>
       </c>
@@ -19794,7 +19830,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="242" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A242" s="1" t="s">
         <v>162</v>
       </c>
@@ -19830,7 +19866,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A243" s="1" t="s">
         <v>162</v>
       </c>
@@ -19866,7 +19902,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="244" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A244" s="1" t="s">
         <v>162</v>
       </c>
@@ -19902,7 +19938,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="245" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A245" s="1" t="s">
         <v>162</v>
       </c>
@@ -19938,7 +19974,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A246" s="1" t="s">
         <v>162</v>
       </c>
@@ -19974,7 +20010,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="247" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A247" s="1" t="s">
         <v>162</v>
       </c>
@@ -20010,7 +20046,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A248" s="1" t="s">
         <v>162</v>
       </c>
@@ -20046,7 +20082,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A249" s="1" t="s">
         <v>162</v>
       </c>
@@ -20082,7 +20118,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A250" s="1" t="s">
         <v>162</v>
       </c>
@@ -20118,7 +20154,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A251" s="1" t="s">
         <v>162</v>
       </c>
@@ -20154,7 +20190,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="252" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A252" s="1" t="s">
         <v>162</v>
       </c>
@@ -20190,7 +20226,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="253" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A253" s="1" t="s">
         <v>162</v>
       </c>
@@ -20226,7 +20262,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="254" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A254" s="1" t="s">
         <v>162</v>
       </c>
@@ -20262,7 +20298,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A255" s="1" t="s">
         <v>162</v>
       </c>
@@ -20298,7 +20334,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A256" s="1" t="s">
         <v>162</v>
       </c>
@@ -20334,7 +20370,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A257" s="1" t="s">
         <v>162</v>
       </c>
@@ -20370,7 +20406,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="258" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A258" s="1" t="s">
         <v>162</v>
       </c>
@@ -20406,7 +20442,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="259" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A259" s="1" t="s">
         <v>162</v>
       </c>
@@ -20442,7 +20478,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="260" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A260" s="1" t="s">
         <v>162</v>
       </c>
@@ -20478,7 +20514,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="261" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A261" s="1" t="s">
         <v>162</v>
       </c>
@@ -20514,7 +20550,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="262" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A262" s="1" t="s">
         <v>162</v>
       </c>
@@ -20550,7 +20586,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A263" s="1" t="s">
         <v>162</v>
       </c>
@@ -20586,7 +20622,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A264" s="1" t="s">
         <v>162</v>
       </c>
@@ -20622,7 +20658,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="265" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A265" s="1" t="s">
         <v>162</v>
       </c>
@@ -20658,7 +20694,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A266" s="1" t="s">
         <v>162</v>
       </c>
@@ -20694,7 +20730,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A267" s="1" t="s">
         <v>162</v>
       </c>
@@ -20730,7 +20766,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="268" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A268" s="1" t="s">
         <v>162</v>
       </c>
@@ -20766,7 +20802,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A269" s="1" t="s">
         <v>162</v>
       </c>
@@ -20802,7 +20838,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A270" s="1" t="s">
         <v>162</v>
       </c>
@@ -20838,7 +20874,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="271" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A271" s="1" t="s">
         <v>162</v>
       </c>
@@ -20874,7 +20910,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="272" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A272" s="1" t="s">
         <v>162</v>
       </c>
@@ -20910,7 +20946,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="273" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A273" s="1" t="s">
         <v>162</v>
       </c>
@@ -20946,7 +20982,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A274" s="1" t="s">
         <v>162</v>
       </c>
@@ -20960,14 +20996,29 @@
         <v>253</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>422</v>
+        <v>877</v>
       </c>
       <c r="F274" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G274" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="H274" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="I274" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="J274" s="9">
+        <v>7</v>
+      </c>
+      <c r="K274" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A275" s="1" t="s">
         <v>162</v>
       </c>
@@ -21003,7 +21054,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A276" s="1" t="s">
         <v>162</v>
       </c>
@@ -21023,8 +21074,23 @@
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G276" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="H276" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="I276" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="J276" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="K276" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A277" s="1" t="s">
         <v>162</v>
       </c>
@@ -21060,7 +21126,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="278" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A278" s="1" t="s">
         <v>162</v>
       </c>
@@ -21096,7 +21162,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A279" s="1" t="s">
         <v>162</v>
       </c>
@@ -21110,14 +21176,29 @@
         <v>256</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>422</v>
+        <v>873</v>
       </c>
       <c r="F279" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G279" s="3" t="s">
+        <v>888</v>
+      </c>
+      <c r="H279" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="I279" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="J279" s="9">
+        <v>6</v>
+      </c>
+      <c r="K279" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A280" s="1" t="s">
         <v>162</v>
       </c>
@@ -21131,14 +21212,29 @@
         <v>257</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>422</v>
+        <v>877</v>
       </c>
       <c r="F280" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G280" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="H280" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="I280" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="J280" s="9">
+        <v>6</v>
+      </c>
+      <c r="K280" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A281" s="1" t="s">
         <v>162</v>
       </c>
@@ -21152,14 +21248,29 @@
         <v>258</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>422</v>
+        <v>873</v>
       </c>
       <c r="F281" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G281" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="H281" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="I281" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="J281" s="9" t="s">
+        <v>665</v>
+      </c>
+      <c r="K281" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A282" s="1" t="s">
         <v>162</v>
       </c>
@@ -21173,14 +21284,29 @@
         <v>259</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>422</v>
+        <v>877</v>
       </c>
       <c r="F282" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G282" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="H282" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="I282" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="J282" s="9">
+        <v>6</v>
+      </c>
+      <c r="K282" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A283" s="1" t="s">
         <v>162</v>
       </c>
@@ -21201,7 +21327,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A284" s="1" t="s">
         <v>162</v>
       </c>
@@ -21222,7 +21348,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A285" s="1" t="s">
         <v>162</v>
       </c>
@@ -21258,7 +21384,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="286" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A286" s="1" t="s">
         <v>162</v>
       </c>
@@ -21294,7 +21420,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A287" s="1" t="s">
         <v>162</v>
       </c>
@@ -21315,7 +21441,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A288" s="1" t="s">
         <v>162</v>
       </c>
@@ -21336,7 +21462,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A289" s="1" t="s">
         <v>162</v>
       </c>
@@ -21357,7 +21483,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A290" s="1" t="s">
         <v>162</v>
       </c>
@@ -21393,7 +21519,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A291" s="1" t="s">
         <v>162</v>
       </c>
@@ -21414,7 +21540,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="292" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A292" s="1" t="s">
         <v>162</v>
       </c>
@@ -21450,7 +21576,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A293" s="1" t="s">
         <v>162</v>
       </c>
@@ -21471,7 +21597,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A294" s="1" t="s">
         <v>162</v>
       </c>
@@ -21492,7 +21618,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A295" s="1" t="s">
         <v>162</v>
       </c>
@@ -21513,7 +21639,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A296" s="1" t="s">
         <v>162</v>
       </c>
@@ -21534,7 +21660,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A297" s="1" t="s">
         <v>162</v>
       </c>
@@ -21555,7 +21681,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A298" s="1" t="s">
         <v>162</v>
       </c>
@@ -21576,7 +21702,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A299" s="1" t="s">
         <v>162</v>
       </c>
@@ -21612,7 +21738,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A300" s="1" t="s">
         <v>162</v>
       </c>
@@ -21648,7 +21774,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="301" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A301" s="1" t="s">
         <v>162</v>
       </c>
@@ -21669,7 +21795,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A302" s="1" t="s">
         <v>162</v>
       </c>
@@ -21690,7 +21816,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="303" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A303" s="1" t="s">
         <v>162</v>
       </c>
@@ -21711,7 +21837,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="304" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A304" s="1" t="s">
         <v>162</v>
       </c>
@@ -21732,7 +21858,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A305" s="1" t="s">
         <v>162</v>
       </c>
@@ -21768,7 +21894,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="306" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A306" s="1" t="s">
         <v>162</v>
       </c>
@@ -21789,7 +21915,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A307" s="1" t="s">
         <v>162</v>
       </c>
@@ -21810,7 +21936,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="308" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A308" s="1" t="s">
         <v>162</v>
       </c>
@@ -21831,7 +21957,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="309" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A309" s="1" t="s">
         <v>162</v>
       </c>
@@ -21867,7 +21993,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="310" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A310" s="1" t="s">
         <v>162</v>
       </c>
@@ -21888,7 +22014,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="311" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A311" s="1" t="s">
         <v>162</v>
       </c>
@@ -21924,7 +22050,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="312" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A312" s="1" t="s">
         <v>162</v>
       </c>
@@ -21945,7 +22071,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A313" s="1" t="s">
         <v>162</v>
       </c>
@@ -21966,7 +22092,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="314" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A314" s="1" t="s">
         <v>162</v>
       </c>
@@ -22002,7 +22128,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="315" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A315" s="1" t="s">
         <v>162</v>
       </c>
@@ -22023,7 +22149,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="316" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A316" s="1" t="s">
         <v>162</v>
       </c>
@@ -22044,7 +22170,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="317" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A317" s="1" t="s">
         <v>162</v>
       </c>
@@ -22065,7 +22191,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="318" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A318" s="1" t="s">
         <v>162</v>
       </c>
@@ -22086,7 +22212,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="319" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A319" s="1" t="s">
         <v>162</v>
       </c>
@@ -22107,7 +22233,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="320" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A320" s="1" t="s">
         <v>162</v>
       </c>
@@ -22128,7 +22254,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="321" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A321" s="1" t="s">
         <v>162</v>
       </c>
@@ -22149,7 +22275,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="322" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A322" s="1" t="s">
         <v>162</v>
       </c>
@@ -22170,7 +22296,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="323" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A323" s="1" t="s">
         <v>162</v>
       </c>
@@ -22191,7 +22317,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="324" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A324" s="1" t="s">
         <v>162</v>
       </c>
@@ -22212,7 +22338,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="325" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A325" s="1" t="s">
         <v>162</v>
       </c>
@@ -22233,7 +22359,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="326" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A326" s="1" t="s">
         <v>162</v>
       </c>
@@ -22269,7 +22395,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="327" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A327" s="1" t="s">
         <v>162</v>
       </c>
@@ -22290,7 +22416,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="328" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A328" s="1" t="s">
         <v>162</v>
       </c>
@@ -22311,7 +22437,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="329" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A329" s="1" t="s">
         <v>162</v>
       </c>
@@ -22347,7 +22473,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="330" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A330" s="1" t="s">
         <v>162</v>
       </c>
@@ -22368,7 +22494,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="331" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A331" s="1" t="s">
         <v>162</v>
       </c>
@@ -22389,7 +22515,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="332" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A332" s="1" t="s">
         <v>162</v>
       </c>
@@ -22410,7 +22536,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="333" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A333" s="1" t="s">
         <v>162</v>
       </c>
@@ -22431,7 +22557,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="334" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A334" s="1" t="s">
         <v>162</v>
       </c>
@@ -22452,7 +22578,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="335" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A335" s="1" t="s">
         <v>162</v>
       </c>
@@ -22488,7 +22614,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="336" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A336" s="1" t="s">
         <v>162</v>
       </c>
@@ -22509,7 +22635,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="337" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A337" s="1" t="s">
         <v>162</v>
       </c>
@@ -22530,7 +22656,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="338" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A338" s="1" t="s">
         <v>162</v>
       </c>
@@ -22551,7 +22677,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="339" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A339" s="1" t="s">
         <v>162</v>
       </c>
@@ -22587,7 +22713,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="340" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A340" s="1" t="s">
         <v>162</v>
       </c>
@@ -22608,7 +22734,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="341" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A341" s="1" t="s">
         <v>162</v>
       </c>
@@ -22629,7 +22755,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="342" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A342" s="1" t="s">
         <v>162</v>
       </c>
@@ -22650,7 +22776,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="343" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A343" s="1" t="s">
         <v>162</v>
       </c>
@@ -22671,7 +22797,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="344" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A344" s="1" t="s">
         <v>162</v>
       </c>
@@ -22692,7 +22818,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="345" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A345" s="1" t="s">
         <v>162</v>
       </c>
@@ -22713,7 +22839,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="346" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A346" s="1" t="s">
         <v>162</v>
       </c>
@@ -22734,7 +22860,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="347" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A347" s="1" t="s">
         <v>162</v>
       </c>
@@ -22770,7 +22896,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="348" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A348" s="1" t="s">
         <v>162</v>
       </c>
@@ -22791,7 +22917,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="349" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A349" s="1" t="s">
         <v>162</v>
       </c>
@@ -22812,7 +22938,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="350" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" s="1" t="s">
         <v>162</v>
       </c>
@@ -22833,7 +22959,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="351" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A351" s="1" t="s">
         <v>162</v>
       </c>
@@ -22869,7 +22995,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="352" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A352" s="1" t="s">
         <v>162</v>
       </c>
@@ -22890,7 +23016,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="353" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A353" s="1" t="s">
         <v>162</v>
       </c>
@@ -22911,7 +23037,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="354" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A354" s="1" t="s">
         <v>162</v>
       </c>
@@ -22932,7 +23058,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="355" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A355" s="1" t="s">
         <v>162</v>
       </c>
@@ -22953,7 +23079,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="356" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A356" s="1" t="s">
         <v>162</v>
       </c>
@@ -22989,7 +23115,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="357" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A357" s="1" t="s">
         <v>162</v>
       </c>
@@ -23010,7 +23136,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="358" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A358" s="1" t="s">
         <v>162</v>
       </c>
@@ -23031,7 +23157,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="359" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A359" s="1" t="s">
         <v>162</v>
       </c>
@@ -23052,7 +23178,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="360" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A360" s="1" t="s">
         <v>162</v>
       </c>
@@ -23088,7 +23214,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="361" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A361" s="1" t="s">
         <v>162</v>
       </c>
@@ -23109,7 +23235,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="362" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A362" s="1" t="s">
         <v>162</v>
       </c>
@@ -23130,7 +23256,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="363" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A363" s="1" t="s">
         <v>162</v>
       </c>
@@ -23151,7 +23277,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="364" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A364" s="1" t="s">
         <v>162</v>
       </c>
@@ -23172,7 +23298,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="365" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A365" s="1" t="s">
         <v>162</v>
       </c>
@@ -23193,7 +23319,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="366" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A366" s="1" t="s">
         <v>162</v>
       </c>
@@ -23214,7 +23340,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="367" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A367" s="1" t="s">
         <v>162</v>
       </c>
@@ -23235,7 +23361,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="368" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A368" s="1" t="s">
         <v>162</v>
       </c>
@@ -23271,7 +23397,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="369" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A369" s="1" t="s">
         <v>162</v>
       </c>
@@ -23292,7 +23418,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="370" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A370" s="1" t="s">
         <v>162</v>
       </c>
@@ -23313,7 +23439,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="371" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A371" s="1" t="s">
         <v>162</v>
       </c>
@@ -23334,7 +23460,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="372" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A372" s="1" t="s">
         <v>162</v>
       </c>
@@ -23370,7 +23496,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="373" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A373" s="1" t="s">
         <v>162</v>
       </c>
@@ -23391,7 +23517,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="374" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A374" s="1" t="s">
         <v>162</v>
       </c>
@@ -23412,7 +23538,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="375" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A375" s="1" t="s">
         <v>162</v>
       </c>
@@ -23433,7 +23559,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="376" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A376" s="1" t="s">
         <v>162</v>
       </c>
@@ -23454,7 +23580,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="377" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A377" s="1" t="s">
         <v>162</v>
       </c>
@@ -23475,7 +23601,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="378" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A378" s="1" t="s">
         <v>162</v>
       </c>
@@ -23496,7 +23622,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="379" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A379" s="1" t="s">
         <v>162</v>
       </c>
@@ -23517,7 +23643,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="380" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A380" s="1" t="s">
         <v>162</v>
       </c>
@@ -23553,7 +23679,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="381" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A381" s="1" t="s">
         <v>162</v>
       </c>
@@ -23574,7 +23700,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="382" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A382" s="1" t="s">
         <v>162</v>
       </c>
@@ -23595,7 +23721,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="383" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A383" s="1" t="s">
         <v>162</v>
       </c>
@@ -23631,7 +23757,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="384" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A384" s="1" t="s">
         <v>162</v>
       </c>
@@ -23667,7 +23793,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="385" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A385" s="1" t="s">
         <v>162</v>
       </c>
@@ -23703,7 +23829,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="386" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A386" s="1" t="s">
         <v>162</v>
       </c>
@@ -23739,7 +23865,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="387" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A387" s="1" t="s">
         <v>162</v>
       </c>
@@ -23775,7 +23901,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="388" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A388" s="1" t="s">
         <v>162</v>
       </c>
@@ -23811,7 +23937,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="389" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A389" s="1" t="s">
         <v>162</v>
       </c>
@@ -23847,7 +23973,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A390" s="1" t="s">
         <v>162</v>
       </c>
@@ -23883,7 +24009,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="391" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A391" s="1" t="s">
         <v>162</v>
       </c>
@@ -23919,7 +24045,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="392" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A392" s="1" t="s">
         <v>162</v>
       </c>
@@ -23955,7 +24081,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="393" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A393" s="1" t="s">
         <v>162</v>
       </c>
@@ -23991,7 +24117,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="394" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A394" s="1" t="s">
         <v>162</v>
       </c>
@@ -24027,7 +24153,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="395" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A395" s="1" t="s">
         <v>162</v>
       </c>
@@ -24063,7 +24189,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="396" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A396" s="1" t="s">
         <v>162</v>
       </c>
@@ -24099,7 +24225,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="397" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A397" s="1" t="s">
         <v>162</v>
       </c>
@@ -24135,7 +24261,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="398" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A398" s="1" t="s">
         <v>162</v>
       </c>
@@ -24171,7 +24297,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="399" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A399" s="1" t="s">
         <v>162</v>
       </c>
@@ -24207,7 +24333,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="400" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A400" s="1" t="s">
         <v>162</v>
       </c>
@@ -24243,7 +24369,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="401" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A401" s="1" t="s">
         <v>162</v>
       </c>
@@ -24279,7 +24405,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="402" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A402" s="1" t="s">
         <v>162</v>
       </c>
@@ -24315,7 +24441,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="403" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A403" s="1" t="s">
         <v>162</v>
       </c>
@@ -24351,7 +24477,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="404" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A404" s="1" t="s">
         <v>162</v>
       </c>
@@ -24387,7 +24513,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="405" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A405" s="1" t="s">
         <v>162</v>
       </c>
@@ -24423,7 +24549,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="406" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A406" s="1" t="s">
         <v>162</v>
       </c>
@@ -24459,7 +24585,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="407" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A407" s="1" t="s">
         <v>162</v>
       </c>
@@ -24495,7 +24621,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="408" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A408" s="1" t="s">
         <v>162</v>
       </c>
@@ -24516,7 +24642,7 @@
         <v>Non</v>
       </c>
     </row>
-    <row r="409" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A409" s="1" t="s">
         <v>162</v>
       </c>
@@ -24552,7 +24678,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="410" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A410" s="1" t="s">
         <v>162</v>
       </c>
@@ -24588,7 +24714,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="411" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A411" s="1" t="s">
         <v>162</v>
       </c>
@@ -24624,7 +24750,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="412" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A412" s="1" t="s">
         <v>162</v>
       </c>
@@ -24660,7 +24786,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="413" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A413" s="1" t="s">
         <v>162</v>
       </c>
@@ -24696,7 +24822,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="414" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A414" s="1" t="s">
         <v>162</v>
       </c>
@@ -24732,7 +24858,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="415" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A415" s="1" t="s">
         <v>162</v>
       </c>
@@ -24768,7 +24894,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="416" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A416" s="1" t="s">
         <v>162</v>
       </c>
@@ -24804,7 +24930,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="417" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A417" s="1" t="s">
         <v>162</v>
       </c>
@@ -24840,7 +24966,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="418" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A418" s="1" t="s">
         <v>162</v>
       </c>
@@ -24876,7 +25002,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="419" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A419" s="1" t="s">
         <v>162</v>
       </c>
@@ -24912,7 +25038,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="420" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A420" s="1" t="s">
         <v>162</v>
       </c>
@@ -24948,7 +25074,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="421" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A421" s="1" t="s">
         <v>162</v>
       </c>
@@ -24984,7 +25110,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="422" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A422" s="1" t="s">
         <v>162</v>
       </c>
@@ -25041,15 +25167,15 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>159</v>
       </c>
@@ -25063,7 +25189,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>160</v>
       </c>
@@ -25077,7 +25203,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -25091,7 +25217,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -25105,7 +25231,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -25119,7 +25245,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>161</v>
       </c>
@@ -25133,7 +25259,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -25147,7 +25273,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -25161,7 +25287,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>161</v>
       </c>
@@ -25175,7 +25301,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>162</v>
       </c>
@@ -25189,7 +25315,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>162</v>
       </c>
@@ -25203,7 +25329,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>162</v>
       </c>
@@ -25217,7 +25343,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>162</v>
       </c>
@@ -25231,7 +25357,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>162</v>
       </c>
@@ -25248,7 +25374,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -25265,7 +25391,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>162</v>
       </c>
@@ -25273,7 +25399,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>162</v>
       </c>
@@ -25281,7 +25407,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>162</v>
       </c>
@@ -25292,7 +25418,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -25301,7 +25427,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>162</v>
       </c>
@@ -25310,7 +25436,7 @@
       </c>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -25324,7 +25450,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>162</v>
       </c>

</xml_diff>

<commit_message>
plus que Seigneurs de l'Ombre a faire
</commit_message>
<xml_diff>
--- a/Liste de dons LG Apocalypse.xlsx
+++ b/Liste de dons LG Apocalypse.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8F10CC-43EE-4FDB-B0EC-0D4FF8BC133F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF90F77D-3B96-4D2B-9468-079CD3CE8E72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="6533" windowWidth="20468" windowHeight="6547" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Repartition thèmes par liste" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3695" uniqueCount="985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3782" uniqueCount="1011">
   <si>
     <t>Liste</t>
   </si>
@@ -2854,9 +2854,6 @@
     <t>L'Ithaeur apprends l'interdit et le fléau de l'esprit</t>
   </si>
   <si>
-    <t>Homicide ?</t>
-  </si>
-  <si>
     <t>La cible humaine aura peur de la nature au point de la laisser intacte</t>
   </si>
   <si>
@@ -2896,9 +2893,6 @@
     <t>Permet de stocker de la Rage, Gnose ou Volonté (à choisir lors de l'acquisition)</t>
   </si>
   <si>
-    <t>Prédation ?</t>
-  </si>
-  <si>
     <t>Homicide</t>
   </si>
   <si>
@@ -2986,12 +2980,6 @@
     <t>Permet d'envoyer un message sur n'importe quel appareil electronique</t>
   </si>
   <si>
-    <t>Toile?</t>
-  </si>
-  <si>
-    <t>Toile ?</t>
-  </si>
-  <si>
     <t>Invoque une Araignée du réseau</t>
   </si>
   <si>
@@ -2999,6 +2987,96 @@
   </si>
   <si>
     <t>Permet d'utiliser la Rage et la Gnose dans le même tour sans pénalités</t>
+  </si>
+  <si>
+    <t>fait une bouillie nutritive à partir de n'importe quoi</t>
+  </si>
+  <si>
+    <t>En réalisant un tour de force (page 270) le LG peut ajouter des dès en échange de dégâts</t>
+  </si>
+  <si>
+    <t>Après avoir touché sa cible le LG la rends mielleuse, elle a une odeur sucrée et est légerement collante. Elle attire des insectes qui lui collent et la dérangent</t>
+  </si>
+  <si>
+    <t>1 heure par réussite</t>
+  </si>
+  <si>
+    <t>Répare temporairement tout objet cassé</t>
+  </si>
+  <si>
+    <t>Survie, poubelles ?</t>
+  </si>
+  <si>
+    <t>Amplifie son musc jusqu'à ce qu'il suffoque ses adversaires</t>
+  </si>
+  <si>
+    <t>Permet de trouver un lieu inhabité par l'humain dans un centre urbain (usines désafectées, appartements abandonnés, etc.)</t>
+  </si>
+  <si>
+    <t>Astuce + Connaissance de la rue</t>
+  </si>
+  <si>
+    <t>Le LG se plonge dans la frénésie pour se battre et augmente ses dégâts</t>
+  </si>
+  <si>
+    <t>La forme lupus du LG resemble à un chien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rouille le métal à proximité </t>
+  </si>
+  <si>
+    <t>Projette son musc sur ses adversaires pour les dégouter au point de les faire vomir</t>
+  </si>
+  <si>
+    <t>Pourrit le bois et le papier</t>
+  </si>
+  <si>
+    <t>Intelligence + Artisanats</t>
+  </si>
+  <si>
+    <t>Résiste aux contrôles mentaux</t>
+  </si>
+  <si>
+    <t>Tant qu'il rit tout haut</t>
+  </si>
+  <si>
+    <t>Plonge dans un coin sombre pour en sortir dans un autre à quelque distance</t>
+  </si>
+  <si>
+    <t>Invoque une horde de vermines</t>
+  </si>
+  <si>
+    <t>Manipulation + Animaux</t>
+  </si>
+  <si>
+    <t>Invoque une horde d'esprits malveillants qui poussent les habitants à faire une émeute</t>
+  </si>
+  <si>
+    <t>Le LG n'a plus besoin de se nourrir, boire ou même respirer. Les températures ne l'affectent plus, etc.</t>
+  </si>
+  <si>
+    <t>Poubelles</t>
+  </si>
+  <si>
+    <t>Domination, orage, secrets</t>
+  </si>
+  <si>
+    <t>Secret ?</t>
+  </si>
+  <si>
+    <t>Toile</t>
+  </si>
+  <si>
+    <t>Entends très bien les chuchotements à proximité</t>
+  </si>
+  <si>
+    <t>Le LG a une aura de supériorité qui l'empêche les autres de lui trouver des défauts</t>
+  </si>
+  <si>
+    <t>Le LG trouve la faiblesse de l'adversaire pour l'utiliser au combat</t>
+  </si>
+  <si>
+    <t>Perception + Empathie</t>
   </si>
 </sst>
 </file>
@@ -11657,8 +11735,8 @@
   <dimension ref="A1:K422"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A336" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D346" sqref="D346"/>
+      <pane ySplit="1" topLeftCell="A363" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A366" sqref="A366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22049,7 +22127,7 @@
         <v>264</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>895</v>
+        <v>915</v>
       </c>
       <c r="F289" s="1" t="str">
         <f t="shared" si="4"/>
@@ -22193,7 +22271,7 @@
         <v>266</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>895</v>
+        <v>915</v>
       </c>
       <c r="F293" s="1" t="str">
         <f t="shared" si="4"/>
@@ -22265,7 +22343,7 @@
         <v>268</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>895</v>
+        <v>915</v>
       </c>
       <c r="F295" s="1" t="str">
         <f t="shared" si="4"/>
@@ -22301,7 +22379,7 @@
         <v>269</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>895</v>
+        <v>915</v>
       </c>
       <c r="F296" s="1" t="str">
         <f t="shared" si="4"/>
@@ -22337,7 +22415,7 @@
         <v>270</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>895</v>
+        <v>915</v>
       </c>
       <c r="F297" s="1" t="str">
         <f t="shared" si="4"/>
@@ -22589,14 +22667,14 @@
         <v>274</v>
       </c>
       <c r="E304" s="1" t="s">
-        <v>936</v>
+        <v>949</v>
       </c>
       <c r="F304" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
       <c r="G304" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="H304" s="1" t="s">
         <v>387</v>
@@ -22608,7 +22686,7 @@
         <v>484</v>
       </c>
       <c r="K304" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
@@ -22668,7 +22746,7 @@
         <v>Oui</v>
       </c>
       <c r="G306" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="H306" s="1" t="s">
         <v>387</v>
@@ -22704,13 +22782,13 @@
         <v>Oui</v>
       </c>
       <c r="G307" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="H307" s="1" t="s">
         <v>387</v>
       </c>
       <c r="I307" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="J307" s="9">
         <v>7</v>
@@ -22733,14 +22811,14 @@
         <v>277</v>
       </c>
       <c r="E308" s="1" t="s">
-        <v>936</v>
+        <v>949</v>
       </c>
       <c r="F308" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
       <c r="G308" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="H308" s="1" t="s">
         <v>387</v>
@@ -22752,7 +22830,7 @@
         <v>484</v>
       </c>
       <c r="K308" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="309" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
@@ -22805,14 +22883,14 @@
         <v>278</v>
       </c>
       <c r="E310" s="1" t="s">
-        <v>936</v>
+        <v>949</v>
       </c>
       <c r="F310" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
       <c r="G310" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H310" s="1" t="s">
         <v>387</v>
@@ -22877,14 +22955,14 @@
         <v>279</v>
       </c>
       <c r="E312" s="1" t="s">
-        <v>936</v>
+        <v>949</v>
       </c>
       <c r="F312" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
       <c r="G312" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H312" s="1" t="s">
         <v>387</v>
@@ -22920,13 +22998,13 @@
         <v>Oui</v>
       </c>
       <c r="G313" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="H313" s="1" t="s">
         <v>420</v>
       </c>
       <c r="I313" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="J313" s="9">
         <v>6</v>
@@ -22992,7 +23070,7 @@
         <v>Oui</v>
       </c>
       <c r="G315" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H315" s="1" t="s">
         <v>387</v>
@@ -23028,7 +23106,7 @@
         <v>Oui</v>
       </c>
       <c r="G316" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H316" s="1" t="s">
         <v>387</v>
@@ -23064,7 +23142,7 @@
         <v>Oui</v>
       </c>
       <c r="G317" s="3" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="H317" s="1" t="s">
         <v>387</v>
@@ -23100,7 +23178,7 @@
         <v>Oui</v>
       </c>
       <c r="G318" s="3" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="H318" s="1" t="s">
         <v>420</v>
@@ -23129,20 +23207,20 @@
         <v>286</v>
       </c>
       <c r="E319" s="1" t="s">
-        <v>936</v>
+        <v>949</v>
       </c>
       <c r="F319" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
       <c r="G319" s="3" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="H319" s="1" t="s">
         <v>420</v>
       </c>
       <c r="I319" s="1" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="J319" s="9">
         <v>7</v>
@@ -23165,14 +23243,14 @@
         <v>287</v>
       </c>
       <c r="E320" s="1" t="s">
-        <v>936</v>
+        <v>949</v>
       </c>
       <c r="F320" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Oui</v>
       </c>
       <c r="G320" s="3" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="H320" s="1" t="s">
         <v>420</v>
@@ -23208,7 +23286,7 @@
         <v>Oui</v>
       </c>
       <c r="G321" s="3" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="H321" s="3" t="s">
         <v>665</v>
@@ -23244,7 +23322,7 @@
         <v>Oui</v>
       </c>
       <c r="G322" s="3" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="H322" s="1" t="s">
         <v>387</v>
@@ -23280,7 +23358,7 @@
         <v>Oui</v>
       </c>
       <c r="G323" s="3" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="H323" s="1" t="s">
         <v>387</v>
@@ -23316,7 +23394,7 @@
         <v>Oui</v>
       </c>
       <c r="G324" s="3" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H324" s="1" t="s">
         <v>393</v>
@@ -23352,7 +23430,7 @@
         <v>Oui</v>
       </c>
       <c r="G325" s="3" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="H325" s="1" t="s">
         <v>420</v>
@@ -23417,14 +23495,14 @@
         <v>296</v>
       </c>
       <c r="E327" s="1" t="s">
-        <v>981</v>
+        <v>1006</v>
       </c>
       <c r="F327" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
       <c r="G327" s="3" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="H327" s="1" t="s">
         <v>393</v>
@@ -23460,7 +23538,7 @@
         <v>Oui</v>
       </c>
       <c r="G328" s="3" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="H328" s="1" t="s">
         <v>420</v>
@@ -23532,13 +23610,13 @@
         <v>Oui</v>
       </c>
       <c r="G330" s="3" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="H330" s="1" t="s">
         <v>393</v>
       </c>
       <c r="I330" s="1" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="J330" s="9">
         <v>7</v>
@@ -23568,7 +23646,7 @@
         <v>Oui</v>
       </c>
       <c r="G331" s="3" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="H331" s="1" t="s">
         <v>420</v>
@@ -23604,13 +23682,13 @@
         <v>Oui</v>
       </c>
       <c r="G332" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="H332" s="1" t="s">
         <v>420</v>
       </c>
       <c r="I332" s="1" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="J332" s="9">
         <v>7</v>
@@ -23640,13 +23718,13 @@
         <v>Oui</v>
       </c>
       <c r="G333" s="3" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="H333" s="1" t="s">
         <v>393</v>
       </c>
       <c r="I333" s="1" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="J333" s="9">
         <v>8</v>
@@ -23676,10 +23754,10 @@
         <v>Oui</v>
       </c>
       <c r="G334" s="3" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="H334" s="1" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="I334" s="1" t="s">
         <v>384</v>
@@ -23748,7 +23826,7 @@
         <v>Oui</v>
       </c>
       <c r="G336" s="3" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="H336" s="1" t="s">
         <v>420</v>
@@ -23760,7 +23838,7 @@
         <v>7</v>
       </c>
       <c r="K336" s="3" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="337" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
@@ -23777,17 +23855,17 @@
         <v>305</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>981</v>
+        <v>1006</v>
       </c>
       <c r="F337" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
       <c r="G337" s="3" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="H337" s="1" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="I337" s="1" t="s">
         <v>384</v>
@@ -23820,7 +23898,7 @@
         <v>Oui</v>
       </c>
       <c r="G338" s="3" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="H338" s="1" t="s">
         <v>420</v>
@@ -23885,14 +23963,14 @@
         <v>307</v>
       </c>
       <c r="E340" s="1" t="s">
-        <v>981</v>
+        <v>1006</v>
       </c>
       <c r="F340" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
       <c r="G340" s="3" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="H340" s="1" t="s">
         <v>420</v>
@@ -23921,20 +23999,20 @@
         <v>309</v>
       </c>
       <c r="E341" s="1" t="s">
-        <v>981</v>
+        <v>1006</v>
       </c>
       <c r="F341" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
       <c r="G341" s="3" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="H341" s="1" t="s">
         <v>420</v>
       </c>
       <c r="I341" s="1" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="J341" s="9">
         <v>8</v>
@@ -23964,7 +24042,7 @@
         <v>Oui</v>
       </c>
       <c r="G342" s="3" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="H342" s="1" t="s">
         <v>387</v>
@@ -23979,7 +24057,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A343" s="1" t="s">
         <v>162</v>
       </c>
@@ -23999,8 +24077,23 @@
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G343" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="H343" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I343" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="J343" s="9">
+        <v>6</v>
+      </c>
+      <c r="K343" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="344" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A344" s="1" t="s">
         <v>162</v>
       </c>
@@ -24020,8 +24113,23 @@
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G344" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="H344" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I344" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="J344" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="K344" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="345" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A345" s="1" t="s">
         <v>162</v>
       </c>
@@ -24035,14 +24143,29 @@
         <v>315</v>
       </c>
       <c r="E345" s="1" t="s">
-        <v>418</v>
+        <v>1003</v>
       </c>
       <c r="F345" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G345" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="H345" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="I345" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="J345" s="9">
+        <v>7</v>
+      </c>
+      <c r="K345" s="3" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="346" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A346" s="1" t="s">
         <v>162</v>
       </c>
@@ -24056,14 +24179,29 @@
         <v>316</v>
       </c>
       <c r="E346" s="1" t="s">
-        <v>418</v>
+        <v>1003</v>
       </c>
       <c r="F346" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="347" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="G346" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="H346" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I346" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="J346" s="9">
+        <v>6</v>
+      </c>
+      <c r="K346" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="347" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A347" s="1" t="s">
         <v>162</v>
       </c>
@@ -24099,7 +24237,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A348" s="1" t="s">
         <v>162</v>
       </c>
@@ -24113,14 +24251,29 @@
         <v>317</v>
       </c>
       <c r="E348" s="1" t="s">
-        <v>418</v>
+        <v>1003</v>
       </c>
       <c r="F348" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G348" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="H348" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="I348" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="J348" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="K348" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="349" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A349" s="1" t="s">
         <v>162</v>
       </c>
@@ -24134,14 +24287,29 @@
         <v>318</v>
       </c>
       <c r="E349" s="1" t="s">
-        <v>418</v>
+        <v>313</v>
       </c>
       <c r="F349" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G349" s="3" t="s">
+        <v>988</v>
+      </c>
+      <c r="H349" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="I349" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="J349" s="9">
+        <v>5</v>
+      </c>
+      <c r="K349" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="350" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" s="1" t="s">
         <v>162</v>
       </c>
@@ -24161,8 +24329,23 @@
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G350" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="H350" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="I350" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="J350" s="9">
+        <v>8</v>
+      </c>
+      <c r="K350" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="351" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A351" s="1" t="s">
         <v>162</v>
       </c>
@@ -24198,7 +24381,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A352" s="1" t="s">
         <v>162</v>
       </c>
@@ -24212,14 +24395,29 @@
         <v>320</v>
       </c>
       <c r="E352" s="1" t="s">
-        <v>418</v>
+        <v>588</v>
       </c>
       <c r="F352" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G352" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="H352" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I352" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="J352" s="9">
+        <v>7</v>
+      </c>
+      <c r="K352" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="353" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A353" s="1" t="s">
         <v>162</v>
       </c>
@@ -24233,14 +24431,29 @@
         <v>321</v>
       </c>
       <c r="E353" s="1" t="s">
-        <v>418</v>
+        <v>1003</v>
       </c>
       <c r="F353" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G353" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="H353" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="I353" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="J353" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="K353" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="354" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A354" s="1" t="s">
         <v>162</v>
       </c>
@@ -24254,14 +24467,29 @@
         <v>322</v>
       </c>
       <c r="E354" s="1" t="s">
-        <v>418</v>
+        <v>1003</v>
       </c>
       <c r="F354" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G354" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="H354" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I354" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="J354" s="9">
+        <v>7</v>
+      </c>
+      <c r="K354" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="355" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A355" s="1" t="s">
         <v>162</v>
       </c>
@@ -24275,14 +24503,29 @@
         <v>323</v>
       </c>
       <c r="E355" s="1" t="s">
-        <v>418</v>
+        <v>1003</v>
       </c>
       <c r="F355" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G355" s="3" t="s">
+        <v>994</v>
+      </c>
+      <c r="H355" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="I355" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="J355" s="9">
+        <v>7</v>
+      </c>
+      <c r="K355" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="356" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A356" s="1" t="s">
         <v>162</v>
       </c>
@@ -24318,7 +24561,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A357" s="1" t="s">
         <v>162</v>
       </c>
@@ -24338,8 +24581,23 @@
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G357" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="H357" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I357" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="J357" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="K357" s="3" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="358" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A358" s="1" t="s">
         <v>162</v>
       </c>
@@ -24359,8 +24617,23 @@
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G358" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="H358" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="I358" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="J358" s="9">
+        <v>6</v>
+      </c>
+      <c r="K358" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="359" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A359" s="1" t="s">
         <v>162</v>
       </c>
@@ -24374,14 +24647,29 @@
         <v>326</v>
       </c>
       <c r="E359" s="1" t="s">
-        <v>418</v>
+        <v>1003</v>
       </c>
       <c r="F359" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="360" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="G359" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="H359" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="I359" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="J359" s="9">
+        <v>7</v>
+      </c>
+      <c r="K359" s="3" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="360" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A360" s="1" t="s">
         <v>162</v>
       </c>
@@ -24417,7 +24705,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A361" s="1" t="s">
         <v>162</v>
       </c>
@@ -24437,8 +24725,23 @@
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="G361" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H361" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="I361" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="J361" s="9">
+        <v>8</v>
+      </c>
+      <c r="K361" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="362" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A362" s="1" t="s">
         <v>162</v>
       </c>
@@ -24458,8 +24761,23 @@
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="363" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="G362" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H362" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="I362" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="J362" s="9">
+        <v>6</v>
+      </c>
+      <c r="K362" s="3" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="363" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A363" s="1" t="s">
         <v>162</v>
       </c>
@@ -24473,14 +24791,29 @@
         <v>330</v>
       </c>
       <c r="E363" s="1" t="s">
-        <v>418</v>
+        <v>1005</v>
       </c>
       <c r="F363" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="364" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="G363" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="H363" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="I363" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="J363" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="K363" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="364" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A364" s="1" t="s">
         <v>162</v>
       </c>
@@ -24494,14 +24827,29 @@
         <v>331</v>
       </c>
       <c r="E364" s="1" t="s">
-        <v>418</v>
+        <v>683</v>
       </c>
       <c r="F364" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="365" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="G364" s="3" t="s">
+        <v>1008</v>
+      </c>
+      <c r="H364" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I364" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="J364" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="K364" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A365" s="1" t="s">
         <v>162</v>
       </c>
@@ -24521,8 +24869,23 @@
         <f t="shared" si="5"/>
         <v>Oui</v>
       </c>
-    </row>
-    <row r="366" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="G365" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H365" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I365" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="J365" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="K365" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="366" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A366" s="1" t="s">
         <v>162</v>
       </c>
@@ -24543,7 +24906,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="367" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A367" s="1" t="s">
         <v>162</v>
       </c>
@@ -24564,7 +24927,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="368" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A368" s="1" t="s">
         <v>162</v>
       </c>
@@ -24600,7 +24963,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="369" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A369" s="1" t="s">
         <v>162</v>
       </c>
@@ -24621,7 +24984,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="370" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A370" s="1" t="s">
         <v>162</v>
       </c>
@@ -24642,7 +25005,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="371" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A371" s="1" t="s">
         <v>162</v>
       </c>
@@ -24663,7 +25026,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="372" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A372" s="1" t="s">
         <v>162</v>
       </c>
@@ -24699,7 +25062,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="373" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A373" s="1" t="s">
         <v>162</v>
       </c>
@@ -24720,7 +25083,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="374" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A374" s="1" t="s">
         <v>162</v>
       </c>
@@ -24741,7 +25104,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="375" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A375" s="1" t="s">
         <v>162</v>
       </c>
@@ -24762,7 +25125,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="376" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A376" s="1" t="s">
         <v>162</v>
       </c>
@@ -24783,7 +25146,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="377" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A377" s="1" t="s">
         <v>162</v>
       </c>
@@ -24804,7 +25167,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="378" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A378" s="1" t="s">
         <v>162</v>
       </c>
@@ -24825,7 +25188,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="379" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A379" s="1" t="s">
         <v>162</v>
       </c>
@@ -24846,7 +25209,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="380" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A380" s="1" t="s">
         <v>162</v>
       </c>
@@ -24882,7 +25245,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="381" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A381" s="1" t="s">
         <v>162</v>
       </c>
@@ -24903,7 +25266,7 @@
         <v>Oui</v>
       </c>
     </row>
-    <row r="382" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A382" s="1" t="s">
         <v>162</v>
       </c>
@@ -25838,7 +26201,7 @@
         <v>246</v>
       </c>
       <c r="E408" s="1" t="s">
-        <v>864</v>
+        <v>883</v>
       </c>
       <c r="F408" s="1" t="str">
         <f t="shared" si="6"/>
@@ -26353,7 +26716,7 @@
   <autoFilter ref="A1:K422" xr:uid="{0A2BBA6B-F0F3-49A4-829D-3714ACDA9F1D}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Rongeurs d'Os"/>
+        <filter val="Seigneurs de l'Ombre"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -26366,8 +26729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35BA778-DA30-4EA6-A9D5-58601F95069A}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26619,10 +26982,10 @@
         <v>273</v>
       </c>
       <c r="C17" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D17" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="E17" t="s">
         <v>916</v>
@@ -26636,7 +26999,7 @@
         <v>290</v>
       </c>
       <c r="C18" t="s">
-        <v>980</v>
+        <v>1006</v>
       </c>
       <c r="D18" t="s">
         <v>293</v>
@@ -26649,10 +27012,18 @@
       <c r="A19" t="s">
         <v>162</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D19" t="s">
+        <v>313</v>
+      </c>
+      <c r="E19" t="s">
+        <v>986</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
@@ -26662,6 +27033,9 @@
         <v>329</v>
       </c>
       <c r="C20" s="8"/>
+      <c r="E20" t="s">
+        <v>1004</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">

</xml_diff>

<commit_message>
commit avant les congés
</commit_message>
<xml_diff>
--- a/Liste de dons LG Apocalypse.xlsx
+++ b/Liste de dons LG Apocalypse.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1CEB1858-1C7B-414D-8452-542C9515F9A3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0336F049-A091-4EFA-AF56-A7BA97DFCF69}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17025" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17025" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Repartition thèmes par liste" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4357" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4356" uniqueCount="1032">
   <si>
     <t>Liste</t>
   </si>
@@ -3122,9 +3122,6 @@
     <t>Donne un nombre de points de Volonté à ses compagnons de meute égal à son score de Gloire. Ces points de Volonté disparaissent à la fin de scène s'ils ne sont pas utilisés.</t>
   </si>
   <si>
-    <t>1scène</t>
-  </si>
-  <si>
     <t>Astuce + Commandement</t>
   </si>
   <si>
@@ -3134,20 +3131,17 @@
     <t>A l'activation de ce Donc les attaques du LG infligent des dégâts sans blesser l'adversaire. Une fois la cible hors combat elle se soigne de toutes ses blessures</t>
   </si>
   <si>
-    <t>Chair commune</t>
-  </si>
-  <si>
-    <t>Transfére des dégâts de ses compagnons de meute sur soit. Le LG peut transférer ainsi un nombre de dégâts égal à son score de pureté par scène.</t>
-  </si>
-  <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>Le LG peut se soigner au milieu d'une bataille sans avoir à s'arrêter un tour pour le faire. Le nombre de blessures qu'il peut se soigner par scène grace à ce Don est égal à sa Pureté.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3165,14 +3159,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3258,7 +3244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -12389,11 +12375,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K422"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="A155" sqref="A155:XFD155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12447,7 +12434,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>160</v>
       </c>
@@ -12483,7 +12470,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>160</v>
       </c>
@@ -12519,7 +12506,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>160</v>
       </c>
@@ -12555,7 +12542,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>160</v>
       </c>
@@ -12591,7 +12578,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
@@ -12627,7 +12614,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>160</v>
       </c>
@@ -12663,7 +12650,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>160</v>
       </c>
@@ -12699,7 +12686,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>160</v>
       </c>
@@ -12735,7 +12722,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>160</v>
       </c>
@@ -12771,7 +12758,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>160</v>
       </c>
@@ -12807,7 +12794,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>160</v>
       </c>
@@ -12843,7 +12830,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>160</v>
       </c>
@@ -12879,7 +12866,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>160</v>
       </c>
@@ -12915,7 +12902,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>160</v>
       </c>
@@ -12951,7 +12938,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>160</v>
       </c>
@@ -12987,7 +12974,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>160</v>
       </c>
@@ -13023,7 +13010,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>160</v>
       </c>
@@ -13059,7 +13046,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>160</v>
       </c>
@@ -13095,7 +13082,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>160</v>
       </c>
@@ -13131,7 +13118,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>160</v>
       </c>
@@ -13167,7 +13154,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>160</v>
       </c>
@@ -13203,7 +13190,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>160</v>
       </c>
@@ -13239,7 +13226,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="14" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>160</v>
       </c>
@@ -13275,7 +13262,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>160</v>
       </c>
@@ -13311,7 +13298,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>160</v>
       </c>
@@ -13347,7 +13334,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>160</v>
       </c>
@@ -13380,7 +13367,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>160</v>
       </c>
@@ -13416,7 +13403,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>160</v>
       </c>
@@ -13449,7 +13436,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>160</v>
       </c>
@@ -13485,7 +13472,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>160</v>
       </c>
@@ -13521,7 +13508,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>160</v>
       </c>
@@ -13557,7 +13544,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>160</v>
       </c>
@@ -13593,7 +13580,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>160</v>
       </c>
@@ -13629,7 +13616,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>160</v>
       </c>
@@ -13665,7 +13652,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>160</v>
       </c>
@@ -13701,7 +13688,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>160</v>
       </c>
@@ -13737,7 +13724,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="14" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>160</v>
       </c>
@@ -13773,7 +13760,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>160</v>
       </c>
@@ -13809,7 +13796,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>160</v>
       </c>
@@ -13845,7 +13832,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>160</v>
       </c>
@@ -13881,7 +13868,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>160</v>
       </c>
@@ -13917,7 +13904,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>160</v>
       </c>
@@ -13953,7 +13940,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>160</v>
       </c>
@@ -13989,7 +13976,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>160</v>
       </c>
@@ -14025,7 +14012,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>160</v>
       </c>
@@ -14061,7 +14048,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>160</v>
       </c>
@@ -14097,7 +14084,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>160</v>
       </c>
@@ -14133,7 +14120,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>160</v>
       </c>
@@ -14169,7 +14156,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>160</v>
       </c>
@@ -14205,7 +14192,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>160</v>
       </c>
@@ -14241,7 +14228,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>160</v>
       </c>
@@ -14277,7 +14264,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>160</v>
       </c>
@@ -14313,7 +14300,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>160</v>
       </c>
@@ -14349,7 +14336,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>160</v>
       </c>
@@ -14385,7 +14372,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>160</v>
       </c>
@@ -14421,7 +14408,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>160</v>
       </c>
@@ -14457,7 +14444,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>160</v>
       </c>
@@ -14493,7 +14480,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>160</v>
       </c>
@@ -14529,7 +14516,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>160</v>
       </c>
@@ -14565,7 +14552,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>160</v>
       </c>
@@ -14601,7 +14588,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>161</v>
       </c>
@@ -14637,7 +14624,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>161</v>
       </c>
@@ -14673,7 +14660,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>161</v>
       </c>
@@ -14709,7 +14696,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>161</v>
       </c>
@@ -14745,7 +14732,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>161</v>
       </c>
@@ -14781,7 +14768,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>161</v>
       </c>
@@ -14817,7 +14804,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>161</v>
       </c>
@@ -14853,7 +14840,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>161</v>
       </c>
@@ -14889,7 +14876,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>161</v>
       </c>
@@ -14925,7 +14912,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>161</v>
       </c>
@@ -14961,7 +14948,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>161</v>
       </c>
@@ -14997,7 +14984,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>161</v>
       </c>
@@ -15033,7 +15020,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>161</v>
       </c>
@@ -15069,7 +15056,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>161</v>
       </c>
@@ -15105,7 +15092,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>161</v>
       </c>
@@ -15141,7 +15128,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>161</v>
       </c>
@@ -15177,7 +15164,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>161</v>
       </c>
@@ -15213,7 +15200,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>161</v>
       </c>
@@ -15249,7 +15236,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>161</v>
       </c>
@@ -15285,7 +15272,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>161</v>
       </c>
@@ -15321,7 +15308,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>161</v>
       </c>
@@ -15357,7 +15344,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>161</v>
       </c>
@@ -15393,7 +15380,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>161</v>
       </c>
@@ -15429,7 +15416,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>161</v>
       </c>
@@ -15465,7 +15452,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>161</v>
       </c>
@@ -15501,7 +15488,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>161</v>
       </c>
@@ -15537,7 +15524,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>161</v>
       </c>
@@ -15573,7 +15560,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>161</v>
       </c>
@@ -15609,7 +15596,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>161</v>
       </c>
@@ -15645,7 +15632,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>161</v>
       </c>
@@ -15681,7 +15668,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>161</v>
       </c>
@@ -15717,7 +15704,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>161</v>
       </c>
@@ -15753,7 +15740,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>161</v>
       </c>
@@ -15789,7 +15776,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>161</v>
       </c>
@@ -15825,7 +15812,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>161</v>
       </c>
@@ -15861,7 +15848,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>161</v>
       </c>
@@ -15897,7 +15884,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>161</v>
       </c>
@@ -15933,7 +15920,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>161</v>
       </c>
@@ -15969,7 +15956,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>161</v>
       </c>
@@ -16005,7 +15992,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>161</v>
       </c>
@@ -16041,7 +16028,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="102" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>161</v>
       </c>
@@ -16077,7 +16064,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>161</v>
       </c>
@@ -16113,7 +16100,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>161</v>
       </c>
@@ -16149,7 +16136,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>161</v>
       </c>
@@ -16185,7 +16172,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>161</v>
       </c>
@@ -16221,7 +16208,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>161</v>
       </c>
@@ -16257,7 +16244,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>161</v>
       </c>
@@ -16293,7 +16280,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>161</v>
       </c>
@@ -16329,7 +16316,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>161</v>
       </c>
@@ -16365,7 +16352,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>161</v>
       </c>
@@ -16401,7 +16388,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>161</v>
       </c>
@@ -16437,7 +16424,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>161</v>
       </c>
@@ -16473,7 +16460,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>161</v>
       </c>
@@ -16509,7 +16496,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>161</v>
       </c>
@@ -16545,7 +16532,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>161</v>
       </c>
@@ -16581,7 +16568,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>161</v>
       </c>
@@ -16617,7 +16604,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>161</v>
       </c>
@@ -16653,7 +16640,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>161</v>
       </c>
@@ -16686,7 +16673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>161</v>
       </c>
@@ -16722,7 +16709,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>161</v>
       </c>
@@ -16758,7 +16745,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>161</v>
       </c>
@@ -16794,7 +16781,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>161</v>
       </c>
@@ -16830,7 +16817,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>161</v>
       </c>
@@ -16866,7 +16853,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>161</v>
       </c>
@@ -16902,7 +16889,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>161</v>
       </c>
@@ -16938,7 +16925,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>161</v>
       </c>
@@ -16974,7 +16961,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>161</v>
       </c>
@@ -17010,7 +16997,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>161</v>
       </c>
@@ -17046,7 +17033,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>161</v>
       </c>
@@ -17082,7 +17069,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>161</v>
       </c>
@@ -17118,7 +17105,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>161</v>
       </c>
@@ -17154,7 +17141,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>161</v>
       </c>
@@ -17190,7 +17177,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>161</v>
       </c>
@@ -17226,7 +17213,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>161</v>
       </c>
@@ -17262,7 +17249,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>161</v>
       </c>
@@ -17298,7 +17285,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>161</v>
       </c>
@@ -17334,7 +17321,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>161</v>
       </c>
@@ -17370,7 +17357,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>161</v>
       </c>
@@ -17406,7 +17393,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>161</v>
       </c>
@@ -17442,7 +17429,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>161</v>
       </c>
@@ -17478,7 +17465,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>161</v>
       </c>
@@ -17514,7 +17501,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>161</v>
       </c>
@@ -17550,7 +17537,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="144" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
         <v>161</v>
       </c>
@@ -17586,7 +17573,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="145" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
         <v>161</v>
       </c>
@@ -17622,7 +17609,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>161</v>
       </c>
@@ -17658,7 +17645,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="147" spans="1:11" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" s="14" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
         <v>161</v>
       </c>
@@ -17694,7 +17681,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>161</v>
       </c>
@@ -17730,7 +17717,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="149" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
         <v>161</v>
       </c>
@@ -17766,7 +17753,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>161</v>
       </c>
@@ -17802,7 +17789,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>161</v>
       </c>
@@ -17838,7 +17825,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>161</v>
       </c>
@@ -17874,7 +17861,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="153" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
         <v>161</v>
       </c>
@@ -17910,7 +17897,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="154" spans="1:11" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" s="14" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
         <v>161</v>
       </c>
@@ -17946,43 +17933,43 @@
         <v>674</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
+    <row r="155" spans="1:11" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="B155" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="14">
         <v>3</v>
       </c>
-      <c r="D155" s="1" t="s">
+      <c r="D155" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="E155" s="1" t="s">
+      <c r="E155" s="14" t="s">
         <v>830</v>
       </c>
-      <c r="F155" s="1" t="str">
+      <c r="F155" s="14" t="str">
         <f t="shared" si="2"/>
         <v>Oui</v>
       </c>
-      <c r="G155" s="3" t="s">
+      <c r="G155" s="15" t="s">
         <v>761</v>
       </c>
-      <c r="H155" s="1" t="s">
+      <c r="H155" s="14" t="s">
         <v>387</v>
       </c>
-      <c r="I155" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="J155" s="9" t="s">
-        <v>384</v>
-      </c>
-      <c r="K155" s="3" t="s">
+      <c r="I155" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="J155" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="K155" s="15" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>161</v>
       </c>
@@ -18018,7 +18005,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>161</v>
       </c>
@@ -18054,7 +18041,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="158" spans="1:11" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" s="14" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
         <v>161</v>
       </c>
@@ -18090,7 +18077,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="159" spans="1:11" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" s="14" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
         <v>161</v>
       </c>
@@ -18126,7 +18113,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>161</v>
       </c>
@@ -18162,7 +18149,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>161</v>
       </c>
@@ -18234,7 +18221,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>162</v>
       </c>
@@ -18270,7 +18257,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
@@ -18306,7 +18293,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>162</v>
       </c>
@@ -18342,7 +18329,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>162</v>
       </c>
@@ -18378,7 +18365,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>162</v>
       </c>
@@ -18414,7 +18401,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>162</v>
       </c>
@@ -18450,7 +18437,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>162</v>
       </c>
@@ -18486,7 +18473,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>162</v>
       </c>
@@ -18522,7 +18509,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="171" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>162</v>
       </c>
@@ -18558,7 +18545,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>162</v>
       </c>
@@ -18594,7 +18581,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>162</v>
       </c>
@@ -18630,7 +18617,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>162</v>
       </c>
@@ -18666,7 +18653,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>162</v>
       </c>
@@ -18702,7 +18689,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>162</v>
       </c>
@@ -18738,7 +18725,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>162</v>
       </c>
@@ -18774,7 +18761,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>162</v>
       </c>
@@ -18810,7 +18797,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>162</v>
       </c>
@@ -18846,7 +18833,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>162</v>
       </c>
@@ -18882,7 +18869,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>162</v>
       </c>
@@ -18918,7 +18905,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>162</v>
       </c>
@@ -18954,7 +18941,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>162</v>
       </c>
@@ -18990,7 +18977,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>162</v>
       </c>
@@ -19026,7 +19013,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>162</v>
       </c>
@@ -19062,7 +19049,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>162</v>
       </c>
@@ -19098,7 +19085,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>162</v>
       </c>
@@ -19134,7 +19121,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>162</v>
       </c>
@@ -19170,7 +19157,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>162</v>
       </c>
@@ -19206,7 +19193,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>162</v>
       </c>
@@ -19242,7 +19229,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>162</v>
       </c>
@@ -19278,7 +19265,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>162</v>
       </c>
@@ -19314,7 +19301,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>162</v>
       </c>
@@ -19350,7 +19337,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>162</v>
       </c>
@@ -19371,7 +19358,7 @@
         <v>Oui</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="H194" s="1" t="s">
         <v>420</v>
@@ -19386,7 +19373,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>162</v>
       </c>
@@ -19422,7 +19409,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>162</v>
       </c>
@@ -19458,7 +19445,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>162</v>
       </c>
@@ -19494,7 +19481,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="198" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>162</v>
       </c>
@@ -19530,7 +19517,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>162</v>
       </c>
@@ -19566,7 +19553,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>162</v>
       </c>
@@ -19602,7 +19589,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>162</v>
       </c>
@@ -19638,7 +19625,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="202" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>162</v>
       </c>
@@ -19674,7 +19661,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>162</v>
       </c>
@@ -19710,7 +19697,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="204" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="14" t="s">
         <v>162</v>
       </c>
@@ -19746,7 +19733,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>162</v>
       </c>
@@ -19782,7 +19769,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>162</v>
       </c>
@@ -19818,7 +19805,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>162</v>
       </c>
@@ -19854,7 +19841,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>162</v>
       </c>
@@ -19890,7 +19877,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="209" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>162</v>
       </c>
@@ -19926,7 +19913,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>162</v>
       </c>
@@ -19962,7 +19949,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>162</v>
       </c>
@@ -19998,7 +19985,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="212" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>162</v>
       </c>
@@ -20034,7 +20021,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="213" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>162</v>
       </c>
@@ -20070,7 +20057,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="214" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="14" t="s">
         <v>162</v>
       </c>
@@ -20106,7 +20093,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>162</v>
       </c>
@@ -20142,7 +20129,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="216" spans="1:11" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" s="14" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="14" t="s">
         <v>162</v>
       </c>
@@ -20178,7 +20165,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>162</v>
       </c>
@@ -20214,7 +20201,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="218" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>162</v>
       </c>
@@ -20250,7 +20237,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>162</v>
       </c>
@@ -20286,7 +20273,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>162</v>
       </c>
@@ -20322,7 +20309,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="221" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>162</v>
       </c>
@@ -20358,7 +20345,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>162</v>
       </c>
@@ -20394,7 +20381,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>162</v>
       </c>
@@ -20430,7 +20417,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="224" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>162</v>
       </c>
@@ -20451,7 +20438,7 @@
         <v>Oui</v>
       </c>
       <c r="G224" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="H224" s="1" t="s">
         <v>420</v>
@@ -20466,7 +20453,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>162</v>
       </c>
@@ -20502,7 +20489,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>162</v>
       </c>
@@ -20538,7 +20525,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>162</v>
       </c>
@@ -20574,7 +20561,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>162</v>
       </c>
@@ -20610,7 +20597,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="229" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>162</v>
       </c>
@@ -20646,7 +20633,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="230" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>162</v>
       </c>
@@ -20682,7 +20669,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="231" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>162</v>
       </c>
@@ -20718,7 +20705,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>162</v>
       </c>
@@ -20754,7 +20741,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="233" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>162</v>
       </c>
@@ -20790,7 +20777,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>162</v>
       </c>
@@ -20826,7 +20813,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>162</v>
       </c>
@@ -20862,7 +20849,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="236" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>162</v>
       </c>
@@ -20898,7 +20885,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="237" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>162</v>
       </c>
@@ -20934,7 +20921,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="238" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>162</v>
       </c>
@@ -20970,7 +20957,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>162</v>
       </c>
@@ -21006,7 +20993,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>162</v>
       </c>
@@ -21042,7 +21029,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="241" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>162</v>
       </c>
@@ -21078,7 +21065,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="242" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>162</v>
       </c>
@@ -21114,7 +21101,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>162</v>
       </c>
@@ -21150,7 +21137,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="244" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>162</v>
       </c>
@@ -21186,7 +21173,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="245" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>162</v>
       </c>
@@ -21222,7 +21209,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>162</v>
       </c>
@@ -21258,7 +21245,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="247" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>162</v>
       </c>
@@ -21294,7 +21281,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>162</v>
       </c>
@@ -21330,7 +21317,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>162</v>
       </c>
@@ -21366,7 +21353,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>162</v>
       </c>
@@ -21402,7 +21389,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>162</v>
       </c>
@@ -21438,7 +21425,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="252" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>162</v>
       </c>
@@ -21474,7 +21461,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="253" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>162</v>
       </c>
@@ -21510,7 +21497,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="254" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>162</v>
       </c>
@@ -21546,7 +21533,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>162</v>
       </c>
@@ -21582,7 +21569,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>162</v>
       </c>
@@ -21618,7 +21605,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>162</v>
       </c>
@@ -21654,7 +21641,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="258" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>162</v>
       </c>
@@ -21690,7 +21677,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="259" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>162</v>
       </c>
@@ -21726,7 +21713,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="260" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>162</v>
       </c>
@@ -21762,7 +21749,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="261" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>162</v>
       </c>
@@ -21798,7 +21785,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="262" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>162</v>
       </c>
@@ -21834,7 +21821,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="263" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="14" t="s">
         <v>162</v>
       </c>
@@ -21870,7 +21857,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>162</v>
       </c>
@@ -21906,7 +21893,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="265" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>162</v>
       </c>
@@ -21942,7 +21929,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>162</v>
       </c>
@@ -21978,7 +21965,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>162</v>
       </c>
@@ -22014,7 +22001,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="268" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>162</v>
       </c>
@@ -22050,7 +22037,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>162</v>
       </c>
@@ -22086,7 +22073,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>162</v>
       </c>
@@ -22122,7 +22109,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="271" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>162</v>
       </c>
@@ -22158,7 +22145,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="272" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>162</v>
       </c>
@@ -22194,7 +22181,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="273" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>162</v>
       </c>
@@ -22230,7 +22217,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="274" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>162</v>
       </c>
@@ -22266,7 +22253,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>162</v>
       </c>
@@ -22302,7 +22289,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>162</v>
       </c>
@@ -22338,7 +22325,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>162</v>
       </c>
@@ -22374,7 +22361,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="278" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>162</v>
       </c>
@@ -22410,7 +22397,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>162</v>
       </c>
@@ -22446,7 +22433,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>162</v>
       </c>
@@ -22482,7 +22469,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>162</v>
       </c>
@@ -22518,7 +22505,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>162</v>
       </c>
@@ -22554,7 +22541,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>162</v>
       </c>
@@ -22590,7 +22577,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>162</v>
       </c>
@@ -22626,7 +22613,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>162</v>
       </c>
@@ -22662,7 +22649,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="286" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>162</v>
       </c>
@@ -22698,7 +22685,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="287" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>162</v>
       </c>
@@ -22734,7 +22721,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>162</v>
       </c>
@@ -22770,7 +22757,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>162</v>
       </c>
@@ -22806,7 +22793,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>162</v>
       </c>
@@ -22842,7 +22829,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="291" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>162</v>
       </c>
@@ -22878,7 +22865,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="292" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>162</v>
       </c>
@@ -22914,7 +22901,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="293" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>162</v>
       </c>
@@ -22950,7 +22937,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>162</v>
       </c>
@@ -22986,7 +22973,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>162</v>
       </c>
@@ -23022,7 +23009,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="296" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>162</v>
       </c>
@@ -23058,7 +23045,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>162</v>
       </c>
@@ -23094,7 +23081,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>162</v>
       </c>
@@ -23130,7 +23117,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>162</v>
       </c>
@@ -23166,7 +23153,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>162</v>
       </c>
@@ -23202,7 +23189,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>162</v>
       </c>
@@ -23238,7 +23225,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>162</v>
       </c>
@@ -23274,7 +23261,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>162</v>
       </c>
@@ -23310,7 +23297,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="304" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>162</v>
       </c>
@@ -23346,7 +23333,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>162</v>
       </c>
@@ -23382,7 +23369,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="306" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>162</v>
       </c>
@@ -23418,7 +23405,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="307" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>162</v>
       </c>
@@ -23454,7 +23441,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="308" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>162</v>
       </c>
@@ -23490,7 +23477,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="309" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>162</v>
       </c>
@@ -23526,7 +23513,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="310" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>162</v>
       </c>
@@ -23562,7 +23549,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="311" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>162</v>
       </c>
@@ -23598,7 +23585,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>162</v>
       </c>
@@ -23634,7 +23621,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>162</v>
       </c>
@@ -23670,7 +23657,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="314" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>162</v>
       </c>
@@ -23706,7 +23693,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="315" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>162</v>
       </c>
@@ -23742,7 +23729,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="316" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>162</v>
       </c>
@@ -23778,7 +23765,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>162</v>
       </c>
@@ -23814,7 +23801,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>162</v>
       </c>
@@ -23850,7 +23837,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="319" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>162</v>
       </c>
@@ -23886,7 +23873,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>162</v>
       </c>
@@ -23922,7 +23909,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="321" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>162</v>
       </c>
@@ -23958,7 +23945,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="322" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>162</v>
       </c>
@@ -23994,7 +23981,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="323" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>162</v>
       </c>
@@ -24030,7 +24017,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>162</v>
       </c>
@@ -24066,7 +24053,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>162</v>
       </c>
@@ -24102,7 +24089,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>162</v>
       </c>
@@ -24138,7 +24125,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="327" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>162</v>
       </c>
@@ -24174,7 +24161,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="328" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>162</v>
       </c>
@@ -24210,7 +24197,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>162</v>
       </c>
@@ -24246,7 +24233,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>162</v>
       </c>
@@ -24282,7 +24269,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="331" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>162</v>
       </c>
@@ -24318,7 +24305,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>162</v>
       </c>
@@ -24354,7 +24341,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="333" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>162</v>
       </c>
@@ -24390,7 +24377,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>162</v>
       </c>
@@ -24426,7 +24413,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="335" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>162</v>
       </c>
@@ -24462,7 +24449,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="336" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>162</v>
       </c>
@@ -24498,7 +24485,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="337" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>162</v>
       </c>
@@ -24534,7 +24521,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>162</v>
       </c>
@@ -24570,7 +24557,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="339" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>162</v>
       </c>
@@ -24606,7 +24593,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="340" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>162</v>
       </c>
@@ -24642,7 +24629,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>162</v>
       </c>
@@ -24678,7 +24665,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="342" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>162</v>
       </c>
@@ -24714,7 +24701,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="343" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>162</v>
       </c>
@@ -24750,7 +24737,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="344" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>162</v>
       </c>
@@ -24786,7 +24773,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="345" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>162</v>
       </c>
@@ -24822,7 +24809,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>162</v>
       </c>
@@ -24858,7 +24845,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="347" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>162</v>
       </c>
@@ -24894,7 +24881,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="348" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>162</v>
       </c>
@@ -24930,7 +24917,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="349" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>162</v>
       </c>
@@ -24966,7 +24953,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="350" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>162</v>
       </c>
@@ -25002,7 +24989,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>162</v>
       </c>
@@ -25038,7 +25025,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>162</v>
       </c>
@@ -25074,7 +25061,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>162</v>
       </c>
@@ -25110,7 +25097,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="354" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>162</v>
       </c>
@@ -25146,7 +25133,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>162</v>
       </c>
@@ -25182,7 +25169,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>162</v>
       </c>
@@ -25218,7 +25205,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>162</v>
       </c>
@@ -25254,7 +25241,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="358" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>162</v>
       </c>
@@ -25290,7 +25277,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>162</v>
       </c>
@@ -25326,7 +25313,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="360" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>162</v>
       </c>
@@ -25362,7 +25349,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="361" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>162</v>
       </c>
@@ -25398,7 +25385,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="362" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>162</v>
       </c>
@@ -25434,7 +25421,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>162</v>
       </c>
@@ -25470,7 +25457,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="364" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>162</v>
       </c>
@@ -25506,7 +25493,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="365" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>162</v>
       </c>
@@ -25542,7 +25529,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="366" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>162</v>
       </c>
@@ -25578,7 +25565,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="367" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>162</v>
       </c>
@@ -25614,7 +25601,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>162</v>
       </c>
@@ -25650,7 +25637,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>162</v>
       </c>
@@ -25686,7 +25673,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="370" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>162</v>
       </c>
@@ -25722,7 +25709,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="371" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>162</v>
       </c>
@@ -25758,7 +25745,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="372" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>162</v>
       </c>
@@ -25794,7 +25781,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>162</v>
       </c>
@@ -25830,7 +25817,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>162</v>
       </c>
@@ -25866,7 +25853,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="375" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>162</v>
       </c>
@@ -25902,7 +25889,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>162</v>
       </c>
@@ -25938,7 +25925,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>162</v>
       </c>
@@ -25974,7 +25961,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="378" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>162</v>
       </c>
@@ -26010,7 +25997,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>162</v>
       </c>
@@ -26046,7 +26033,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>162</v>
       </c>
@@ -26082,7 +26069,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="381" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>162</v>
       </c>
@@ -26118,7 +26105,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>162</v>
       </c>
@@ -26154,7 +26141,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>162</v>
       </c>
@@ -26190,7 +26177,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>162</v>
       </c>
@@ -26226,7 +26213,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="385" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
         <v>162</v>
       </c>
@@ -26262,7 +26249,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="386" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>162</v>
       </c>
@@ -26298,7 +26285,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="387" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
         <v>162</v>
       </c>
@@ -26334,7 +26321,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="388" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>162</v>
       </c>
@@ -26370,7 +26357,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>162</v>
       </c>
@@ -26406,7 +26393,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="390" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>162</v>
       </c>
@@ -26442,7 +26429,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="391" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>162</v>
       </c>
@@ -26478,7 +26465,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="392" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>162</v>
       </c>
@@ -26514,7 +26501,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="393" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>162</v>
       </c>
@@ -26550,7 +26537,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>162</v>
       </c>
@@ -26586,7 +26573,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>162</v>
       </c>
@@ -26622,7 +26609,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>162</v>
       </c>
@@ -26658,7 +26645,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="397" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>162</v>
       </c>
@@ -26694,7 +26681,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>162</v>
       </c>
@@ -26730,7 +26717,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>162</v>
       </c>
@@ -26766,7 +26753,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="400" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>162</v>
       </c>
@@ -26802,7 +26789,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>162</v>
       </c>
@@ -26838,7 +26825,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>162</v>
       </c>
@@ -26874,7 +26861,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>162</v>
       </c>
@@ -26910,7 +26897,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="404" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>162</v>
       </c>
@@ -26946,7 +26933,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>162</v>
       </c>
@@ -26982,7 +26969,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="406" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>162</v>
       </c>
@@ -27018,7 +27005,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>162</v>
       </c>
@@ -27054,7 +27041,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>162</v>
       </c>
@@ -27075,7 +27062,7 @@
         <v>Non</v>
       </c>
     </row>
-    <row r="409" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>162</v>
       </c>
@@ -27111,7 +27098,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="410" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>162</v>
       </c>
@@ -27147,7 +27134,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>162</v>
       </c>
@@ -27183,7 +27170,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>162</v>
       </c>
@@ -27219,7 +27206,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="413" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>162</v>
       </c>
@@ -27255,7 +27242,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>162</v>
       </c>
@@ -27291,7 +27278,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="415" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>162</v>
       </c>
@@ -27327,7 +27314,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>162</v>
       </c>
@@ -27363,7 +27350,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="417" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>162</v>
       </c>
@@ -27399,7 +27386,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>162</v>
       </c>
@@ -27435,7 +27422,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>162</v>
       </c>
@@ -27471,7 +27458,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="420" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
         <v>162</v>
       </c>
@@ -27507,7 +27494,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="421" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
         <v>162</v>
       </c>
@@ -27543,7 +27530,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
         <v>162</v>
       </c>
@@ -27580,7 +27567,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K422" xr:uid="{0A2BBA6B-F0F3-49A4-829D-3714ACDA9F1D}"/>
+  <autoFilter ref="A1:K422" xr:uid="{0A2BBA6B-F0F3-49A4-829D-3714ACDA9F1D}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Régénération"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -27590,11 +27583,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE07F88F-88EC-40BA-9516-0F3D1085A2BB}">
   <dimension ref="A1:I216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27955,7 +27948,7 @@
         <v>384</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>1027</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -27972,13 +27965,13 @@
         <v>1004</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>1009</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="H13" s="18">
         <v>7</v>
@@ -27987,33 +27980,33 @@
         <v>385</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>762</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>1031</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>1032</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>672</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>1008</v>
+        <v>384</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>1009</v>
+        <v>468</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>384</v>
+        <v>462</v>
+      </c>
+      <c r="H14" s="18">
+        <v>7</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>